<commit_message>
Latest generated outputs 2025-09-10
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/advertising-advertising.xlsx
+++ b/generated/spreadsheet/advertising-advertising.xlsx
@@ -1073,9 +1073,7 @@
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Information about advertisement placement including whether it's already in place,
-replacement status, and potential overhang over public areas
-</t>
+          <t>Where the advertisement being applied to be built will be located</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
@@ -1247,8 +1245,7 @@
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Module for capturing the time period that consent to advertisement is sought
-</t>
+          <t>How long the proposed advertisement will be shown.</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr">
@@ -1308,9 +1305,7 @@
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Module for capturing information about different types of advertisements 
-proposed, including their counts and descriptions
-</t>
+          <t>What type of advertisements are proposed and how many there will be.</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
@@ -1434,8 +1429,7 @@
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Contact details of the agent acting on behalf of the applicant
-</t>
+          <t>Name and contact information if an agent is being used.</t>
         </is>
       </c>
       <c r="C33" s="2" t="inlineStr">
@@ -1567,8 +1561,7 @@
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Details of the agent acting on behalf of the applicant
-</t>
+          <t>Name and contact information if an agent is being used.</t>
         </is>
       </c>
       <c r="C37" s="2" t="inlineStr">
@@ -1836,8 +1829,7 @@
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Contact details for the applicant or applicants, including email and phone numbers
-</t>
+          <t>Telephone number and email address of the applicant.</t>
         </is>
       </c>
       <c r="C45" s="2" t="inlineStr">
@@ -1969,9 +1961,7 @@
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Details about the applicants for the planning application,
-including their personal information and contact details
-</t>
+          <t>Name and contact information for the parties making the application.</t>
         </is>
       </c>
       <c r="C49" s="2" t="inlineStr">
@@ -2179,8 +2169,7 @@
       </c>
       <c r="B55" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Identifies the national requirement types that apply to this application type
-</t>
+          <t>Checking whether all the requirements of the form have been met, such as proof of payment or supporting documentation.</t>
         </is>
       </c>
       <c r="C55" s="2" t="inlineStr">
@@ -2214,8 +2203,7 @@
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Information about community consultation activities carried out in relation to the planning application
-</t>
+          <t>What community consultation activities have taken place as part of the application</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
@@ -2275,9 +2263,7 @@
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Information about any conflicts of interest between the applicant/agent and the planning authority,
-including relationships with staff or elected members
-</t>
+          <t>Details of any conflict of interest that may exist between the applicant and planning authority.</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr">
@@ -2363,9 +2349,7 @@
       </c>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Details of the applicant's interest in land or listed buildings and information about
-other interested parties including owners and persons with interests in the property
-</t>
+          <t>Names and contact details for all parties with an interest in the proposed develpoment.</t>
         </is>
       </c>
       <c r="C61" s="2" t="inlineStr">
@@ -2937,8 +2921,7 @@
       </c>
       <c r="B79" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Declaration by the applicant or agent confirming the accuracy of the information provided
-</t>
+          <t>Signed and dated verification of the application's accuracy.</t>
         </is>
       </c>
       <c r="C79" s="2" t="inlineStr">
@@ -3024,8 +3007,7 @@
       </c>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Information about any pre-application advice sought from the planning authority
-</t>
+          <t>Details of pre-application advice received from the planning authority</t>
         </is>
       </c>
       <c r="C82" s="2" t="inlineStr">
@@ -3163,7 +3145,7 @@
       </c>
       <c r="B87" s="2" t="inlineStr">
         <is>
-          <t>Details of proposed advertisements including dimensions, materials, and illumination specifications</t>
+          <t>Details of the proposed advertisements such as their size and how they are made</t>
         </is>
       </c>
       <c r="C87" s="2" t="inlineStr">
@@ -3531,9 +3513,7 @@
       </c>
       <c r="B99" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Information about the location and extent of the site where development 
-or works are proposed
-</t>
+          <t>Where the proposed development will be built.</t>
         </is>
       </c>
       <c r="C99" s="2" t="inlineStr">
@@ -3811,8 +3791,7 @@
       </c>
       <c r="B108" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Details needed to support a site visit by the planning authority
-</t>
+          <t>Information to help the planning authority arrange a site visit</t>
         </is>
       </c>
       <c r="C108" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Latest generated outputs 2025-10-28
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/advertising-advertising.xlsx
+++ b/generated/spreadsheet/advertising-advertising.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,9 +440,10 @@
     <col width="36" customWidth="1" min="3" max="3"/>
     <col width="33" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="72" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="72" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -473,15 +474,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>field4</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>datatype</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>requirement</t>
         </is>
@@ -500,22 +506,27 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
           <t>Reference</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr"/>
       <c r="E2" s="2" t="inlineStr"/>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr"/>
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>A unique reference for the data item</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -526,22 +537,27 @@
       <c r="B3" s="2" t="n"/>
       <c r="C3" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
           <t>Application types[]</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr"/>
       <c r="E3" s="2" t="inlineStr"/>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr"/>
+      <c r="G3" s="2" t="inlineStr">
         <is>
           <t>A list of planning application types that define the nature of the planning application</t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr">
+      <c r="H3" s="2" t="inlineStr">
         <is>
           <t>enum</t>
         </is>
       </c>
-      <c r="H3" s="2" t="inlineStr">
+      <c r="I3" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -552,22 +568,27 @@
       <c r="B4" s="2" t="n"/>
       <c r="C4" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
           <t>Application sub type</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr"/>
       <c r="E4" s="2" t="inlineStr"/>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr"/>
+      <c r="G4" s="2" t="inlineStr">
         <is>
           <t>Further classification of the application type for specific variations within the main application type</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
+      <c r="H4" s="2" t="inlineStr">
         <is>
           <t>enum</t>
         </is>
       </c>
-      <c r="H4" s="2" t="inlineStr">
+      <c r="I4" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -578,22 +599,27 @@
       <c r="B5" s="2" t="n"/>
       <c r="C5" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
           <t>Planning authority</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr"/>
       <c r="E5" s="2" t="inlineStr"/>
-      <c r="F5" s="2" t="inlineStr">
+      <c r="F5" s="2" t="inlineStr"/>
+      <c r="G5" s="2" t="inlineStr">
         <is>
           <t>The reference of the planning authority the application has been submitted to, e.g. local-authority:CMD</t>
         </is>
       </c>
-      <c r="G5" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -604,22 +630,27 @@
       <c r="B6" s="2" t="n"/>
       <c r="C6" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
           <t>Submission date</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr"/>
       <c r="E6" s="2" t="inlineStr"/>
-      <c r="F6" s="2" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr"/>
+      <c r="G6" s="2" t="inlineStr">
         <is>
           <t>Date the application is submitted in YYYY-MM-DD format</t>
         </is>
       </c>
-      <c r="G6" s="2" t="inlineStr">
+      <c r="H6" s="2" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="H6" s="2" t="inlineStr">
+      <c r="I6" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -630,22 +661,27 @@
       <c r="B7" s="2" t="n"/>
       <c r="C7" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
           <t>Modules[]</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr"/>
       <c r="E7" s="2" t="inlineStr"/>
-      <c r="F7" s="2" t="inlineStr">
+      <c r="F7" s="2" t="inlineStr"/>
+      <c r="G7" s="2" t="inlineStr">
         <is>
           <t>List of required modules for this application that can be used to validate the application</t>
         </is>
       </c>
-      <c r="G7" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -656,26 +692,31 @@
       <c r="B8" s="2" t="n"/>
       <c r="C8" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
           <t>Documents[]</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>Reference</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr"/>
-      <c r="F8" s="2" t="inlineStr">
+      <c r="F8" s="2" t="inlineStr"/>
+      <c r="G8" s="2" t="inlineStr">
         <is>
           <t>A reference for the document</t>
         </is>
       </c>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -686,26 +727,31 @@
       <c r="B9" s="2" t="n"/>
       <c r="C9" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
           <t>Documents[]</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr"/>
-      <c r="F9" s="2" t="inlineStr">
+      <c r="F9" s="2" t="inlineStr"/>
+      <c r="G9" s="2" t="inlineStr">
         <is>
           <t>The name or title of the document</t>
         </is>
       </c>
-      <c r="G9" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I9" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -716,26 +762,31 @@
       <c r="B10" s="2" t="n"/>
       <c r="C10" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
           <t>Documents[]</t>
         </is>
       </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr"/>
-      <c r="F10" s="2" t="inlineStr">
+      <c r="F10" s="2" t="inlineStr"/>
+      <c r="G10" s="2" t="inlineStr">
         <is>
           <t>Brief description of what the document contains</t>
         </is>
       </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I10" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -746,26 +797,31 @@
       <c r="B11" s="2" t="n"/>
       <c r="C11" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
           <t>Documents[]</t>
         </is>
       </c>
-      <c r="D11" s="2" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>Document types[]</t>
         </is>
       </c>
-      <c r="E11" s="2" t="inlineStr"/>
-      <c r="F11" s="2" t="inlineStr">
+      <c r="F11" s="2" t="inlineStr"/>
+      <c r="G11" s="2" t="inlineStr">
         <is>
           <t>List of codelist references that the document covers</t>
         </is>
       </c>
-      <c r="G11" s="2" t="inlineStr">
+      <c r="H11" s="2" t="inlineStr">
         <is>
           <t>enum</t>
         </is>
       </c>
-      <c r="H11" s="2" t="inlineStr">
+      <c r="I11" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -776,30 +832,35 @@
       <c r="B12" s="2" t="n"/>
       <c r="C12" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
           <t>Documents[]</t>
         </is>
       </c>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>File</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
+      <c r="F12" s="2" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="F12" s="2" t="inlineStr">
+      <c r="G12" s="2" t="inlineStr">
         <is>
           <t>A URL pointing to the stored file</t>
         </is>
       </c>
-      <c r="G12" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H12" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I12" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -810,30 +871,35 @@
       <c r="B13" s="2" t="n"/>
       <c r="C13" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
           <t>Documents[]</t>
         </is>
       </c>
-      <c r="D13" s="2" t="inlineStr">
+      <c r="E13" s="2" t="inlineStr">
         <is>
           <t>File</t>
         </is>
       </c>
-      <c r="E13" s="2" t="inlineStr">
+      <c r="F13" s="2" t="inlineStr">
         <is>
           <t>Base64</t>
         </is>
       </c>
-      <c r="F13" s="2" t="inlineStr">
+      <c r="G13" s="2" t="inlineStr">
         <is>
           <t>Base64-encoded content of the file for inline file uploads</t>
         </is>
       </c>
-      <c r="G13" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H13" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I13" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -844,30 +910,35 @@
       <c r="B14" s="2" t="n"/>
       <c r="C14" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
           <t>Documents[]</t>
         </is>
       </c>
-      <c r="D14" s="2" t="inlineStr">
+      <c r="E14" s="2" t="inlineStr">
         <is>
           <t>File</t>
         </is>
       </c>
-      <c r="E14" s="2" t="inlineStr">
+      <c r="F14" s="2" t="inlineStr">
         <is>
           <t>Filename</t>
         </is>
       </c>
-      <c r="F14" s="2" t="inlineStr">
+      <c r="G14" s="2" t="inlineStr">
         <is>
           <t>Name of the file being uploaded</t>
         </is>
       </c>
-      <c r="G14" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H14" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I14" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -878,30 +949,35 @@
       <c r="B15" s="2" t="n"/>
       <c r="C15" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
           <t>Documents[]</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr">
+      <c r="E15" s="2" t="inlineStr">
         <is>
           <t>File</t>
         </is>
       </c>
-      <c r="E15" s="2" t="inlineStr">
+      <c r="F15" s="2" t="inlineStr">
         <is>
           <t>MIME type</t>
         </is>
       </c>
-      <c r="F15" s="2" t="inlineStr">
+      <c r="G15" s="2" t="inlineStr">
         <is>
           <t>The file's MIME type such as application/pdf or image/jpeg</t>
         </is>
       </c>
-      <c r="G15" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H15" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I15" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -912,30 +988,35 @@
       <c r="B16" s="2" t="n"/>
       <c r="C16" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
           <t>Documents[]</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr">
+      <c r="E16" s="2" t="inlineStr">
         <is>
           <t>File</t>
         </is>
       </c>
-      <c r="E16" s="2" t="inlineStr">
+      <c r="F16" s="2" t="inlineStr">
         <is>
           <t>Checksum</t>
         </is>
       </c>
-      <c r="F16" s="2" t="inlineStr">
+      <c r="G16" s="2" t="inlineStr">
         <is>
           <t>Hash of the file contents used for file validation and checking files have not been tampered with</t>
         </is>
       </c>
-      <c r="G16" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H16" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I16" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -946,30 +1027,35 @@
       <c r="B17" s="2" t="n"/>
       <c r="C17" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
           <t>Documents[]</t>
         </is>
       </c>
-      <c r="D17" s="2" t="inlineStr">
+      <c r="E17" s="2" t="inlineStr">
         <is>
           <t>File</t>
         </is>
       </c>
-      <c r="E17" s="2" t="inlineStr">
+      <c r="F17" s="2" t="inlineStr">
         <is>
           <t>File size</t>
         </is>
       </c>
-      <c r="F17" s="2" t="inlineStr">
+      <c r="G17" s="2" t="inlineStr">
         <is>
           <t>Size of the file in bytes that can be used to enforce limits</t>
         </is>
       </c>
-      <c r="G17" s="2" t="inlineStr">
+      <c r="H17" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H17" s="2" t="inlineStr">
+      <c r="I17" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -980,26 +1066,31 @@
       <c r="B18" s="2" t="n"/>
       <c r="C18" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
           <t>Fee</t>
         </is>
       </c>
-      <c r="D18" s="2" t="inlineStr">
+      <c r="E18" s="2" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="E18" s="2" t="inlineStr"/>
-      <c r="F18" s="2" t="inlineStr">
+      <c r="F18" s="2" t="inlineStr"/>
+      <c r="G18" s="2" t="inlineStr">
         <is>
           <t>The total amount due for the application fee</t>
         </is>
       </c>
-      <c r="G18" s="2" t="inlineStr">
+      <c r="H18" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H18" s="2" t="inlineStr">
+      <c r="I18" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1010,26 +1101,31 @@
       <c r="B19" s="2" t="n"/>
       <c r="C19" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
           <t>Fee</t>
         </is>
       </c>
-      <c r="D19" s="2" t="inlineStr">
+      <c r="E19" s="2" t="inlineStr">
         <is>
           <t>Amount paid</t>
         </is>
       </c>
-      <c r="E19" s="2" t="inlineStr"/>
-      <c r="F19" s="2" t="inlineStr">
+      <c r="F19" s="2" t="inlineStr"/>
+      <c r="G19" s="2" t="inlineStr">
         <is>
           <t>The amount paid towards the application fee</t>
         </is>
       </c>
-      <c r="G19" s="2" t="inlineStr">
+      <c r="H19" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H19" s="2" t="inlineStr">
+      <c r="I19" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1040,26 +1136,31 @@
       <c r="B20" s="2" t="n"/>
       <c r="C20" s="2" t="inlineStr">
         <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
           <t>Fee</t>
         </is>
       </c>
-      <c r="D20" s="2" t="inlineStr">
+      <c r="E20" s="2" t="inlineStr">
         <is>
           <t>Transactions[]</t>
         </is>
       </c>
-      <c r="E20" s="2" t="inlineStr"/>
-      <c r="F20" s="2" t="inlineStr">
+      <c r="F20" s="2" t="inlineStr"/>
+      <c r="G20" s="2" t="inlineStr">
         <is>
           <t>References to payments or financial transactions related to this application</t>
         </is>
       </c>
-      <c r="G20" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H20" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I20" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -1083,17 +1184,18 @@
       </c>
       <c r="D21" s="2" t="inlineStr"/>
       <c r="E21" s="2" t="inlineStr"/>
-      <c r="F21" s="2" t="inlineStr">
+      <c r="F21" s="2" t="inlineStr"/>
+      <c r="G21" s="2" t="inlineStr">
         <is>
           <t>Whether the advertisement is already in place</t>
         </is>
       </c>
-      <c r="G21" s="2" t="inlineStr">
+      <c r="H21" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H21" s="2" t="inlineStr">
+      <c r="I21" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1109,17 +1211,18 @@
       </c>
       <c r="D22" s="2" t="inlineStr"/>
       <c r="E22" s="2" t="inlineStr"/>
-      <c r="F22" s="2" t="inlineStr">
+      <c r="F22" s="2" t="inlineStr"/>
+      <c r="G22" s="2" t="inlineStr">
         <is>
           <t>Date when the advertisement was placed (YYYY-MM-DD format)</t>
         </is>
       </c>
-      <c r="G22" s="2" t="inlineStr">
+      <c r="H22" s="2" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="H22" s="2" t="inlineStr">
+      <c r="I22" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -1135,17 +1238,18 @@
       </c>
       <c r="D23" s="2" t="inlineStr"/>
       <c r="E23" s="2" t="inlineStr"/>
-      <c r="F23" s="2" t="inlineStr">
+      <c r="F23" s="2" t="inlineStr"/>
+      <c r="G23" s="2" t="inlineStr">
         <is>
           <t>Whether this is a replacement advertisement</t>
         </is>
       </c>
-      <c r="G23" s="2" t="inlineStr">
+      <c r="H23" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H23" s="2" t="inlineStr">
+      <c r="I23" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1165,17 +1269,18 @@
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr"/>
-      <c r="F24" s="2" t="inlineStr">
+      <c r="F24" s="2" t="inlineStr"/>
+      <c r="G24" s="2" t="inlineStr">
         <is>
           <t>A unique reference for the data item</t>
         </is>
       </c>
-      <c r="G24" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H24" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I24" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1195,17 +1300,18 @@
         </is>
       </c>
       <c r="E25" s="2" t="inlineStr"/>
-      <c r="F25" s="2" t="inlineStr">
+      <c r="F25" s="2" t="inlineStr"/>
+      <c r="G25" s="2" t="inlineStr">
         <is>
           <t>A name for the document. For example, The Site Plan</t>
         </is>
       </c>
-      <c r="G25" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H25" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I25" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1221,17 +1327,18 @@
       </c>
       <c r="D26" s="2" t="inlineStr"/>
       <c r="E26" s="2" t="inlineStr"/>
-      <c r="F26" s="2" t="inlineStr">
+      <c r="F26" s="2" t="inlineStr"/>
+      <c r="G26" s="2" t="inlineStr">
         <is>
           <t>Whether the advertisement will project over a footpath or other public highway</t>
         </is>
       </c>
-      <c r="G26" s="2" t="inlineStr">
+      <c r="H26" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H26" s="2" t="inlineStr">
+      <c r="I26" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1255,17 +1362,18 @@
       </c>
       <c r="D27" s="2" t="inlineStr"/>
       <c r="E27" s="2" t="inlineStr"/>
-      <c r="F27" s="2" t="inlineStr">
+      <c r="F27" s="2" t="inlineStr"/>
+      <c r="G27" s="2" t="inlineStr">
         <is>
           <t>The start of the time period that consent to advertisement is sought</t>
         </is>
       </c>
-      <c r="G27" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H27" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I27" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1281,17 +1389,18 @@
       </c>
       <c r="D28" s="2" t="inlineStr"/>
       <c r="E28" s="2" t="inlineStr"/>
-      <c r="F28" s="2" t="inlineStr">
+      <c r="F28" s="2" t="inlineStr"/>
+      <c r="G28" s="2" t="inlineStr">
         <is>
           <t>The end of the time period that consent to advertisement is sought</t>
         </is>
       </c>
-      <c r="G28" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H28" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I28" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1315,17 +1424,18 @@
       </c>
       <c r="D29" s="2" t="inlineStr"/>
       <c r="E29" s="2" t="inlineStr"/>
-      <c r="F29" s="2" t="inlineStr">
+      <c r="F29" s="2" t="inlineStr"/>
+      <c r="G29" s="2" t="inlineStr">
         <is>
           <t>Description of the advertisement proposal</t>
         </is>
       </c>
-      <c r="G29" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H29" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I29" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1345,17 +1455,18 @@
         </is>
       </c>
       <c r="E30" s="2" t="inlineStr"/>
-      <c r="F30" s="2" t="inlineStr">
+      <c r="F30" s="2" t="inlineStr"/>
+      <c r="G30" s="2" t="inlineStr">
         <is>
           <t>One of the advertisement-types or other</t>
         </is>
       </c>
-      <c r="G30" s="2" t="inlineStr">
+      <c r="H30" s="2" t="inlineStr">
         <is>
           <t>enum</t>
         </is>
       </c>
-      <c r="H30" s="2" t="inlineStr">
+      <c r="I30" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1375,17 +1486,18 @@
         </is>
       </c>
       <c r="E31" s="2" t="inlineStr"/>
-      <c r="F31" s="2" t="inlineStr">
+      <c r="F31" s="2" t="inlineStr"/>
+      <c r="G31" s="2" t="inlineStr">
         <is>
           <t>Number of this type of advertisement</t>
         </is>
       </c>
-      <c r="G31" s="2" t="inlineStr">
+      <c r="H31" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H31" s="2" t="inlineStr">
+      <c r="I31" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1405,17 +1517,18 @@
         </is>
       </c>
       <c r="E32" s="2" t="inlineStr"/>
-      <c r="F32" s="2" t="inlineStr">
+      <c r="F32" s="2" t="inlineStr"/>
+      <c r="G32" s="2" t="inlineStr">
         <is>
           <t>Details required if other advertisement type is selected</t>
         </is>
       </c>
-      <c r="G32" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H32" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I32" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -1439,17 +1552,18 @@
       </c>
       <c r="D33" s="2" t="inlineStr"/>
       <c r="E33" s="2" t="inlineStr"/>
-      <c r="F33" s="2" t="inlineStr">
+      <c r="F33" s="2" t="inlineStr"/>
+      <c r="G33" s="2" t="inlineStr">
         <is>
           <t>A reference to an agent object</t>
         </is>
       </c>
-      <c r="G33" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H33" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I33" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1469,17 +1583,18 @@
         </is>
       </c>
       <c r="E34" s="2" t="inlineStr"/>
-      <c r="F34" s="2" t="inlineStr">
+      <c r="F34" s="2" t="inlineStr"/>
+      <c r="G34" s="2" t="inlineStr">
         <is>
           <t>The email address that can be used for electronic correspondence with the individual</t>
         </is>
       </c>
-      <c r="G34" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H34" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I34" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1503,17 +1618,18 @@
           <t>Phone number</t>
         </is>
       </c>
-      <c r="F35" s="2" t="inlineStr">
+      <c r="F35" s="2" t="inlineStr"/>
+      <c r="G35" s="2" t="inlineStr">
         <is>
           <t>A phone number</t>
         </is>
       </c>
-      <c r="G35" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H35" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I35" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -1537,17 +1653,18 @@
           <t>Contact priority</t>
         </is>
       </c>
-      <c r="F36" s="2" t="inlineStr">
+      <c r="F36" s="2" t="inlineStr"/>
+      <c r="G36" s="2" t="inlineStr">
         <is>
           <t>The priority of a number</t>
         </is>
       </c>
-      <c r="G36" s="2" t="inlineStr">
+      <c r="H36" s="2" t="inlineStr">
         <is>
           <t>enum</t>
         </is>
       </c>
-      <c r="H36" s="2" t="inlineStr">
+      <c r="I36" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -1575,17 +1692,18 @@
         </is>
       </c>
       <c r="E37" s="2" t="inlineStr"/>
-      <c r="F37" s="2" t="inlineStr">
+      <c r="F37" s="2" t="inlineStr"/>
+      <c r="G37" s="2" t="inlineStr">
         <is>
           <t>A unique reference for the data item</t>
         </is>
       </c>
-      <c r="G37" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H37" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I37" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1609,17 +1727,18 @@
           <t>Title</t>
         </is>
       </c>
-      <c r="F38" s="2" t="inlineStr">
+      <c r="F38" s="2" t="inlineStr"/>
+      <c r="G38" s="2" t="inlineStr">
         <is>
           <t>The title of the individual</t>
         </is>
       </c>
-      <c r="G38" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H38" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I38" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -1643,17 +1762,18 @@
           <t>First Name</t>
         </is>
       </c>
-      <c r="F39" s="2" t="inlineStr">
+      <c r="F39" s="2" t="inlineStr"/>
+      <c r="G39" s="2" t="inlineStr">
         <is>
           <t>The first name of the individual</t>
         </is>
       </c>
-      <c r="G39" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H39" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I39" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1677,17 +1797,18 @@
           <t>Last Name</t>
         </is>
       </c>
-      <c r="F40" s="2" t="inlineStr">
+      <c r="F40" s="2" t="inlineStr"/>
+      <c r="G40" s="2" t="inlineStr">
         <is>
           <t>The last name of the individual</t>
         </is>
       </c>
-      <c r="G40" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H40" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I40" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1711,17 +1832,18 @@
           <t>Address Text</t>
         </is>
       </c>
-      <c r="F41" s="2" t="inlineStr">
+      <c r="F41" s="2" t="inlineStr"/>
+      <c r="G41" s="2" t="inlineStr">
         <is>
           <t>Flexible field for capturing addresses</t>
         </is>
       </c>
-      <c r="G41" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H41" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I41" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1745,17 +1867,18 @@
           <t>Postcode</t>
         </is>
       </c>
-      <c r="F42" s="2" t="inlineStr">
+      <c r="F42" s="2" t="inlineStr"/>
+      <c r="G42" s="2" t="inlineStr">
         <is>
           <t>The postal code</t>
         </is>
       </c>
-      <c r="G42" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H42" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I42" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -1775,17 +1898,18 @@
         </is>
       </c>
       <c r="E43" s="2" t="inlineStr"/>
-      <c r="F43" s="2" t="inlineStr">
+      <c r="F43" s="2" t="inlineStr"/>
+      <c r="G43" s="2" t="inlineStr">
         <is>
           <t>The name of a company (that the agent works for)</t>
         </is>
       </c>
-      <c r="G43" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H43" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I43" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -1805,17 +1929,18 @@
         </is>
       </c>
       <c r="E44" s="2" t="inlineStr"/>
-      <c r="F44" s="2" t="inlineStr">
+      <c r="F44" s="2" t="inlineStr"/>
+      <c r="G44" s="2" t="inlineStr">
         <is>
           <t>The role of the named individual. Agent or proxy</t>
         </is>
       </c>
-      <c r="G44" s="2" t="inlineStr">
+      <c r="H44" s="2" t="inlineStr">
         <is>
           <t>enum</t>
         </is>
       </c>
-      <c r="H44" s="2" t="inlineStr">
+      <c r="I44" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -1839,17 +1964,18 @@
       </c>
       <c r="D45" s="2" t="inlineStr"/>
       <c r="E45" s="2" t="inlineStr"/>
-      <c r="F45" s="2" t="inlineStr">
+      <c r="F45" s="2" t="inlineStr"/>
+      <c r="G45" s="2" t="inlineStr">
         <is>
           <t>Reference to match contact details to a named individual from the applicant details component</t>
         </is>
       </c>
-      <c r="G45" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H45" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I45" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1869,17 +1995,18 @@
         </is>
       </c>
       <c r="E46" s="2" t="inlineStr"/>
-      <c r="F46" s="2" t="inlineStr">
+      <c r="F46" s="2" t="inlineStr"/>
+      <c r="G46" s="2" t="inlineStr">
         <is>
           <t>The email address that can be used for electronic correspondence with the individual</t>
         </is>
       </c>
-      <c r="G46" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H46" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I46" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -1903,17 +2030,18 @@
           <t>Phone number</t>
         </is>
       </c>
-      <c r="F47" s="2" t="inlineStr">
+      <c r="F47" s="2" t="inlineStr"/>
+      <c r="G47" s="2" t="inlineStr">
         <is>
           <t>A phone number</t>
         </is>
       </c>
-      <c r="G47" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H47" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I47" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -1937,17 +2065,18 @@
           <t>Contact priority</t>
         </is>
       </c>
-      <c r="F48" s="2" t="inlineStr">
+      <c r="F48" s="2" t="inlineStr"/>
+      <c r="G48" s="2" t="inlineStr">
         <is>
           <t>The priority of a number</t>
         </is>
       </c>
-      <c r="G48" s="2" t="inlineStr">
+      <c r="H48" s="2" t="inlineStr">
         <is>
           <t>enum</t>
         </is>
       </c>
-      <c r="H48" s="2" t="inlineStr">
+      <c r="I48" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -1975,17 +2104,18 @@
         </is>
       </c>
       <c r="E49" s="2" t="inlineStr"/>
-      <c r="F49" s="2" t="inlineStr">
+      <c r="F49" s="2" t="inlineStr"/>
+      <c r="G49" s="2" t="inlineStr">
         <is>
           <t>A unique reference for the data item</t>
         </is>
       </c>
-      <c r="G49" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H49" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I49" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2009,17 +2139,18 @@
           <t>Title</t>
         </is>
       </c>
-      <c r="F50" s="2" t="inlineStr">
+      <c r="F50" s="2" t="inlineStr"/>
+      <c r="G50" s="2" t="inlineStr">
         <is>
           <t>The title of the individual</t>
         </is>
       </c>
-      <c r="G50" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H50" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I50" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2043,17 +2174,18 @@
           <t>First Name</t>
         </is>
       </c>
-      <c r="F51" s="2" t="inlineStr">
+      <c r="F51" s="2" t="inlineStr"/>
+      <c r="G51" s="2" t="inlineStr">
         <is>
           <t>The first name of the individual</t>
         </is>
       </c>
-      <c r="G51" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H51" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I51" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2077,17 +2209,18 @@
           <t>Last Name</t>
         </is>
       </c>
-      <c r="F52" s="2" t="inlineStr">
+      <c r="F52" s="2" t="inlineStr"/>
+      <c r="G52" s="2" t="inlineStr">
         <is>
           <t>The last name of the individual</t>
         </is>
       </c>
-      <c r="G52" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H52" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I52" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2111,17 +2244,18 @@
           <t>Address Text</t>
         </is>
       </c>
-      <c r="F53" s="2" t="inlineStr">
+      <c r="F53" s="2" t="inlineStr"/>
+      <c r="G53" s="2" t="inlineStr">
         <is>
           <t>Flexible field for capturing addresses</t>
         </is>
       </c>
-      <c r="G53" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H53" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I53" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2145,17 +2279,18 @@
           <t>Postcode</t>
         </is>
       </c>
-      <c r="F54" s="2" t="inlineStr">
+      <c r="F54" s="2" t="inlineStr"/>
+      <c r="G54" s="2" t="inlineStr">
         <is>
           <t>The postal code</t>
         </is>
       </c>
-      <c r="G54" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H54" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I54" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2179,17 +2314,18 @@
       </c>
       <c r="D55" s="2" t="inlineStr"/>
       <c r="E55" s="2" t="inlineStr"/>
-      <c r="F55" s="2" t="inlineStr">
+      <c r="F55" s="2" t="inlineStr"/>
+      <c r="G55" s="2" t="inlineStr">
         <is>
           <t>List of the document types required for the given application type</t>
         </is>
       </c>
-      <c r="G55" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H55" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I55" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2213,17 +2349,18 @@
       </c>
       <c r="D56" s="2" t="inlineStr"/>
       <c r="E56" s="2" t="inlineStr"/>
-      <c r="F56" s="2" t="inlineStr">
+      <c r="F56" s="2" t="inlineStr"/>
+      <c r="G56" s="2" t="inlineStr">
         <is>
           <t>Whether community consultation has been carried out</t>
         </is>
       </c>
-      <c r="G56" s="2" t="inlineStr">
+      <c r="H56" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H56" s="2" t="inlineStr">
+      <c r="I56" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2239,17 +2376,18 @@
       </c>
       <c r="D57" s="2" t="inlineStr"/>
       <c r="E57" s="2" t="inlineStr"/>
-      <c r="F57" s="2" t="inlineStr">
+      <c r="F57" s="2" t="inlineStr"/>
+      <c r="G57" s="2" t="inlineStr">
         <is>
           <t>Provide details of the community consultation</t>
         </is>
       </c>
-      <c r="G57" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H57" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I57" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2273,17 +2411,18 @@
       </c>
       <c r="D58" s="2" t="inlineStr"/>
       <c r="E58" s="2" t="inlineStr"/>
-      <c r="F58" s="2" t="inlineStr">
+      <c r="F58" s="2" t="inlineStr"/>
+      <c r="G58" s="2" t="inlineStr">
         <is>
           <t>Indicates whether any named applicant or agent has a relationship to the planning authority that must be declared</t>
         </is>
       </c>
-      <c r="G58" s="2" t="inlineStr">
+      <c r="H58" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H58" s="2" t="inlineStr">
+      <c r="I58" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2299,17 +2438,18 @@
       </c>
       <c r="D59" s="2" t="inlineStr"/>
       <c r="E59" s="2" t="inlineStr"/>
-      <c r="F59" s="2" t="inlineStr">
+      <c r="F59" s="2" t="inlineStr"/>
+      <c r="G59" s="2" t="inlineStr">
         <is>
           <t>Name of the individual with the conflict of interest that matches one of the names provided in applicants/agent section</t>
         </is>
       </c>
-      <c r="G59" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H59" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I59" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2325,17 +2465,18 @@
       </c>
       <c r="D60" s="2" t="inlineStr"/>
       <c r="E60" s="2" t="inlineStr"/>
-      <c r="F60" s="2" t="inlineStr">
+      <c r="F60" s="2" t="inlineStr"/>
+      <c r="G60" s="2" t="inlineStr">
         <is>
           <t>Details of the conflict of interest including name, role and how the individual is related to the planning authority</t>
         </is>
       </c>
-      <c r="G60" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H60" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I60" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2359,17 +2500,18 @@
       </c>
       <c r="D61" s="2" t="inlineStr"/>
       <c r="E61" s="2" t="inlineStr"/>
-      <c r="F61" s="2" t="inlineStr">
+      <c r="F61" s="2" t="inlineStr"/>
+      <c r="G61" s="2" t="inlineStr">
         <is>
           <t>Description of the applicant's interest in the land</t>
         </is>
       </c>
-      <c r="G61" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H61" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I61" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2393,17 +2535,18 @@
           <t>Title</t>
         </is>
       </c>
-      <c r="F62" s="2" t="inlineStr">
+      <c r="F62" s="2" t="inlineStr"/>
+      <c r="G62" s="2" t="inlineStr">
         <is>
           <t>The title of the individual</t>
         </is>
       </c>
-      <c r="G62" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H62" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I62" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2427,17 +2570,18 @@
           <t>First Name</t>
         </is>
       </c>
-      <c r="F63" s="2" t="inlineStr">
+      <c r="F63" s="2" t="inlineStr"/>
+      <c r="G63" s="2" t="inlineStr">
         <is>
           <t>The first name of the individual</t>
         </is>
       </c>
-      <c r="G63" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H63" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I63" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2461,17 +2605,18 @@
           <t>Last Name</t>
         </is>
       </c>
-      <c r="F64" s="2" t="inlineStr">
+      <c r="F64" s="2" t="inlineStr"/>
+      <c r="G64" s="2" t="inlineStr">
         <is>
           <t>The last name of the individual</t>
         </is>
       </c>
-      <c r="G64" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H64" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I64" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2495,17 +2640,18 @@
           <t>Address Text</t>
         </is>
       </c>
-      <c r="F65" s="2" t="inlineStr">
+      <c r="F65" s="2" t="inlineStr"/>
+      <c r="G65" s="2" t="inlineStr">
         <is>
           <t>Flexible field for capturing addresses</t>
         </is>
       </c>
-      <c r="G65" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H65" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I65" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2529,17 +2675,18 @@
           <t>Postcode</t>
         </is>
       </c>
-      <c r="F66" s="2" t="inlineStr">
+      <c r="F66" s="2" t="inlineStr"/>
+      <c r="G66" s="2" t="inlineStr">
         <is>
           <t>The postal code</t>
         </is>
       </c>
-      <c r="G66" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H66" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I66" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2559,17 +2706,18 @@
         </is>
       </c>
       <c r="E67" s="2" t="inlineStr"/>
-      <c r="F67" s="2" t="inlineStr">
+      <c r="F67" s="2" t="inlineStr"/>
+      <c r="G67" s="2" t="inlineStr">
         <is>
           <t>Whether the owner has been informed of the application</t>
         </is>
       </c>
-      <c r="G67" s="2" t="inlineStr">
+      <c r="H67" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H67" s="2" t="inlineStr">
+      <c r="I67" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2593,17 +2741,18 @@
           <t>Title</t>
         </is>
       </c>
-      <c r="F68" s="2" t="inlineStr">
+      <c r="F68" s="2" t="inlineStr"/>
+      <c r="G68" s="2" t="inlineStr">
         <is>
           <t>The title of the individual</t>
         </is>
       </c>
-      <c r="G68" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H68" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I68" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2627,17 +2776,18 @@
           <t>First Name</t>
         </is>
       </c>
-      <c r="F69" s="2" t="inlineStr">
+      <c r="F69" s="2" t="inlineStr"/>
+      <c r="G69" s="2" t="inlineStr">
         <is>
           <t>The first name of the individual</t>
         </is>
       </c>
-      <c r="G69" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H69" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I69" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2661,17 +2811,18 @@
           <t>Last Name</t>
         </is>
       </c>
-      <c r="F70" s="2" t="inlineStr">
+      <c r="F70" s="2" t="inlineStr"/>
+      <c r="G70" s="2" t="inlineStr">
         <is>
           <t>The last name of the individual</t>
         </is>
       </c>
-      <c r="G70" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H70" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I70" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2695,17 +2846,18 @@
           <t>Address Text</t>
         </is>
       </c>
-      <c r="F71" s="2" t="inlineStr">
+      <c r="F71" s="2" t="inlineStr"/>
+      <c r="G71" s="2" t="inlineStr">
         <is>
           <t>Flexible field for capturing addresses</t>
         </is>
       </c>
-      <c r="G71" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H71" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I71" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2729,17 +2881,18 @@
           <t>Postcode</t>
         </is>
       </c>
-      <c r="F72" s="2" t="inlineStr">
+      <c r="F72" s="2" t="inlineStr"/>
+      <c r="G72" s="2" t="inlineStr">
         <is>
           <t>The postal code</t>
         </is>
       </c>
-      <c r="G72" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H72" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I72" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2759,17 +2912,18 @@
         </is>
       </c>
       <c r="E73" s="2" t="inlineStr"/>
-      <c r="F73" s="2" t="inlineStr">
+      <c r="F73" s="2" t="inlineStr"/>
+      <c r="G73" s="2" t="inlineStr">
         <is>
           <t>Description of the nature of a person's interest in the property</t>
         </is>
       </c>
-      <c r="G73" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H73" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I73" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2789,17 +2943,18 @@
         </is>
       </c>
       <c r="E74" s="2" t="inlineStr"/>
-      <c r="F74" s="2" t="inlineStr">
+      <c r="F74" s="2" t="inlineStr"/>
+      <c r="G74" s="2" t="inlineStr">
         <is>
           <t>Whether the person has been informed of the application</t>
         </is>
       </c>
-      <c r="G74" s="2" t="inlineStr">
+      <c r="H74" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H74" s="2" t="inlineStr">
+      <c r="I74" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2819,17 +2974,18 @@
         </is>
       </c>
       <c r="E75" s="2" t="inlineStr"/>
-      <c r="F75" s="2" t="inlineStr">
+      <c r="F75" s="2" t="inlineStr"/>
+      <c r="G75" s="2" t="inlineStr">
         <is>
           <t>Reason why a person was not informed of the application</t>
         </is>
       </c>
-      <c r="G75" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H75" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I75" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2845,17 +3001,18 @@
       </c>
       <c r="D76" s="2" t="inlineStr"/>
       <c r="E76" s="2" t="inlineStr"/>
-      <c r="F76" s="2" t="inlineStr">
+      <c r="F76" s="2" t="inlineStr"/>
+      <c r="G76" s="2" t="inlineStr">
         <is>
           <t>True or False indicating whether the applicant owns the land where the advertisement will be displayed</t>
         </is>
       </c>
-      <c r="G76" s="2" t="inlineStr">
+      <c r="H76" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H76" s="2" t="inlineStr">
+      <c r="I76" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2871,17 +3028,18 @@
       </c>
       <c r="D77" s="2" t="inlineStr"/>
       <c r="E77" s="2" t="inlineStr"/>
-      <c r="F77" s="2" t="inlineStr">
+      <c r="F77" s="2" t="inlineStr"/>
+      <c r="G77" s="2" t="inlineStr">
         <is>
           <t>True or False indicating whether permission of the owner for the display of an advertisement has been obtained</t>
         </is>
       </c>
-      <c r="G77" s="2" t="inlineStr">
+      <c r="H77" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H77" s="2" t="inlineStr">
+      <c r="I77" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2897,17 +3055,18 @@
       </c>
       <c r="D78" s="2" t="inlineStr"/>
       <c r="E78" s="2" t="inlineStr"/>
-      <c r="F78" s="2" t="inlineStr">
+      <c r="F78" s="2" t="inlineStr"/>
+      <c r="G78" s="2" t="inlineStr">
         <is>
           <t>Details explaining why permission from the land owner has not been obtained for the advertisement display</t>
         </is>
       </c>
-      <c r="G78" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H78" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I78" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -2931,17 +3090,18 @@
       </c>
       <c r="D79" s="2" t="inlineStr"/>
       <c r="E79" s="2" t="inlineStr"/>
-      <c r="F79" s="2" t="inlineStr">
+      <c r="F79" s="2" t="inlineStr"/>
+      <c r="G79" s="2" t="inlineStr">
         <is>
           <t>A name of a person</t>
         </is>
       </c>
-      <c r="G79" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H79" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I79" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2957,17 +3117,18 @@
       </c>
       <c r="D80" s="2" t="inlineStr"/>
       <c r="E80" s="2" t="inlineStr"/>
-      <c r="F80" s="2" t="inlineStr">
+      <c r="F80" s="2" t="inlineStr"/>
+      <c r="G80" s="2" t="inlineStr">
         <is>
           <t>Confirms the applicant or agent has reviewed and validated the information provided in the application</t>
         </is>
       </c>
-      <c r="G80" s="2" t="inlineStr">
+      <c r="H80" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H80" s="2" t="inlineStr">
+      <c r="I80" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -2983,17 +3144,18 @@
       </c>
       <c r="D81" s="2" t="inlineStr"/>
       <c r="E81" s="2" t="inlineStr"/>
-      <c r="F81" s="2" t="inlineStr">
+      <c r="F81" s="2" t="inlineStr"/>
+      <c r="G81" s="2" t="inlineStr">
         <is>
           <t>The date the declaration was made</t>
         </is>
       </c>
-      <c r="G81" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H81" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I81" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -3017,17 +3179,18 @@
       </c>
       <c r="D82" s="2" t="inlineStr"/>
       <c r="E82" s="2" t="inlineStr"/>
-      <c r="F82" s="2" t="inlineStr">
+      <c r="F82" s="2" t="inlineStr"/>
+      <c r="G82" s="2" t="inlineStr">
         <is>
           <t>Whether pre-application advice has been sought from the planning authority</t>
         </is>
       </c>
-      <c r="G82" s="2" t="inlineStr">
+      <c r="H82" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H82" s="2" t="inlineStr">
+      <c r="I82" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -3043,17 +3206,18 @@
       </c>
       <c r="D83" s="2" t="inlineStr"/>
       <c r="E83" s="2" t="inlineStr"/>
-      <c r="F83" s="2" t="inlineStr">
+      <c r="F83" s="2" t="inlineStr"/>
+      <c r="G83" s="2" t="inlineStr">
         <is>
           <t>Name of the planning officer who provided the pre-application advice</t>
         </is>
       </c>
-      <c r="G83" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H83" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I83" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3069,17 +3233,18 @@
       </c>
       <c r="D84" s="2" t="inlineStr"/>
       <c r="E84" s="2" t="inlineStr"/>
-      <c r="F84" s="2" t="inlineStr">
+      <c r="F84" s="2" t="inlineStr"/>
+      <c r="G84" s="2" t="inlineStr">
         <is>
           <t>A unique reference for the data item</t>
         </is>
       </c>
-      <c r="G84" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H84" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I84" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3095,17 +3260,18 @@
       </c>
       <c r="D85" s="2" t="inlineStr"/>
       <c r="E85" s="2" t="inlineStr"/>
-      <c r="F85" s="2" t="inlineStr">
+      <c r="F85" s="2" t="inlineStr"/>
+      <c r="G85" s="2" t="inlineStr">
         <is>
           <t>Date when pre-application advice was received, in YYYY-MM-DD format</t>
         </is>
       </c>
-      <c r="G85" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H85" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I85" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3121,17 +3287,18 @@
       </c>
       <c r="D86" s="2" t="inlineStr"/>
       <c r="E86" s="2" t="inlineStr"/>
-      <c r="F86" s="2" t="inlineStr">
+      <c r="F86" s="2" t="inlineStr"/>
+      <c r="G86" s="2" t="inlineStr">
         <is>
           <t>Summary of the pre-application advice received from the planning authority</t>
         </is>
       </c>
-      <c r="G86" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H86" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I86" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3159,17 +3326,18 @@
         </is>
       </c>
       <c r="E87" s="2" t="inlineStr"/>
-      <c r="F87" s="2" t="inlineStr">
+      <c r="F87" s="2" t="inlineStr"/>
+      <c r="G87" s="2" t="inlineStr">
         <is>
           <t>Height, in metres, from ground to the base of the advertisement</t>
         </is>
       </c>
-      <c r="G87" s="2" t="inlineStr">
+      <c r="H87" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H87" s="2" t="inlineStr">
+      <c r="I87" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3189,17 +3357,18 @@
         </is>
       </c>
       <c r="E88" s="2" t="inlineStr"/>
-      <c r="F88" s="2" t="inlineStr">
+      <c r="F88" s="2" t="inlineStr"/>
+      <c r="G88" s="2" t="inlineStr">
         <is>
           <t>Height, in metres, of dimensions of advertisement</t>
         </is>
       </c>
-      <c r="G88" s="2" t="inlineStr">
+      <c r="H88" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H88" s="2" t="inlineStr">
+      <c r="I88" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3219,17 +3388,18 @@
         </is>
       </c>
       <c r="E89" s="2" t="inlineStr"/>
-      <c r="F89" s="2" t="inlineStr">
+      <c r="F89" s="2" t="inlineStr"/>
+      <c r="G89" s="2" t="inlineStr">
         <is>
           <t>Width of dimensions of advertisement</t>
         </is>
       </c>
-      <c r="G89" s="2" t="inlineStr">
+      <c r="H89" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H89" s="2" t="inlineStr">
+      <c r="I89" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3249,17 +3419,18 @@
         </is>
       </c>
       <c r="E90" s="2" t="inlineStr"/>
-      <c r="F90" s="2" t="inlineStr">
+      <c r="F90" s="2" t="inlineStr"/>
+      <c r="G90" s="2" t="inlineStr">
         <is>
           <t>Depth, in metres, of dimensions of advertisement</t>
         </is>
       </c>
-      <c r="G90" s="2" t="inlineStr">
+      <c r="H90" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H90" s="2" t="inlineStr">
+      <c r="I90" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3279,17 +3450,18 @@
         </is>
       </c>
       <c r="E91" s="2" t="inlineStr"/>
-      <c r="F91" s="2" t="inlineStr">
+      <c r="F91" s="2" t="inlineStr"/>
+      <c r="G91" s="2" t="inlineStr">
         <is>
           <t>Maximum height, in metres, of any individual letters or symbols</t>
         </is>
       </c>
-      <c r="G91" s="2" t="inlineStr">
+      <c r="H91" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H91" s="2" t="inlineStr">
+      <c r="I91" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3309,17 +3481,18 @@
         </is>
       </c>
       <c r="E92" s="2" t="inlineStr"/>
-      <c r="F92" s="2" t="inlineStr">
+      <c r="F92" s="2" t="inlineStr"/>
+      <c r="G92" s="2" t="inlineStr">
         <is>
           <t>Colour of proposed sign</t>
         </is>
       </c>
-      <c r="G92" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H92" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I92" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3339,17 +3512,18 @@
         </is>
       </c>
       <c r="E93" s="2" t="inlineStr"/>
-      <c r="F93" s="2" t="inlineStr">
+      <c r="F93" s="2" t="inlineStr"/>
+      <c r="G93" s="2" t="inlineStr">
         <is>
           <t>Materials of proposed sign</t>
         </is>
       </c>
-      <c r="G93" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H93" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I93" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3369,17 +3543,18 @@
         </is>
       </c>
       <c r="E94" s="2" t="inlineStr"/>
-      <c r="F94" s="2" t="inlineStr">
+      <c r="F94" s="2" t="inlineStr"/>
+      <c r="G94" s="2" t="inlineStr">
         <is>
           <t>Maximum projection, in metres, of the advertisement from the face of the building</t>
         </is>
       </c>
-      <c r="G94" s="2" t="inlineStr">
+      <c r="H94" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H94" s="2" t="inlineStr">
+      <c r="I94" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3399,17 +3574,18 @@
         </is>
       </c>
       <c r="E95" s="2" t="inlineStr"/>
-      <c r="F95" s="2" t="inlineStr">
+      <c r="F95" s="2" t="inlineStr"/>
+      <c r="G95" s="2" t="inlineStr">
         <is>
           <t>Will the sign(s) be illuminated?</t>
         </is>
       </c>
-      <c r="G95" s="2" t="inlineStr">
+      <c r="H95" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H95" s="2" t="inlineStr">
+      <c r="I95" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3429,17 +3605,18 @@
         </is>
       </c>
       <c r="E96" s="2" t="inlineStr"/>
-      <c r="F96" s="2" t="inlineStr">
+      <c r="F96" s="2" t="inlineStr"/>
+      <c r="G96" s="2" t="inlineStr">
         <is>
           <t>Method of illumination for the advertisement</t>
         </is>
       </c>
-      <c r="G96" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H96" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I96" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3459,17 +3636,18 @@
         </is>
       </c>
       <c r="E97" s="2" t="inlineStr"/>
-      <c r="F97" s="2" t="inlineStr">
+      <c r="F97" s="2" t="inlineStr"/>
+      <c r="G97" s="2" t="inlineStr">
         <is>
           <t>Level of illuminance for the advertisement</t>
         </is>
       </c>
-      <c r="G97" s="2" t="inlineStr">
+      <c r="H97" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H97" s="2" t="inlineStr">
+      <c r="I97" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3489,17 +3667,18 @@
         </is>
       </c>
       <c r="E98" s="2" t="inlineStr"/>
-      <c r="F98" s="2" t="inlineStr">
+      <c r="F98" s="2" t="inlineStr"/>
+      <c r="G98" s="2" t="inlineStr">
         <is>
           <t>Type of illumination (static or intermittent)</t>
         </is>
       </c>
-      <c r="G98" s="2" t="inlineStr">
+      <c r="H98" s="2" t="inlineStr">
         <is>
           <t>enum</t>
         </is>
       </c>
-      <c r="H98" s="2" t="inlineStr">
+      <c r="I98" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3527,17 +3706,18 @@
         </is>
       </c>
       <c r="E99" s="2" t="inlineStr"/>
-      <c r="F99" s="2" t="inlineStr">
+      <c r="F99" s="2" t="inlineStr"/>
+      <c r="G99" s="2" t="inlineStr">
         <is>
           <t>Geometry of the site of the development, typically in GeoJSON format</t>
         </is>
       </c>
-      <c r="G99" s="2" t="inlineStr">
+      <c r="H99" s="2" t="inlineStr">
         <is>
           <t>wkt</t>
         </is>
       </c>
-      <c r="H99" s="2" t="inlineStr">
+      <c r="I99" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3557,17 +3737,18 @@
         </is>
       </c>
       <c r="E100" s="2" t="inlineStr"/>
-      <c r="F100" s="2" t="inlineStr">
+      <c r="F100" s="2" t="inlineStr"/>
+      <c r="G100" s="2" t="inlineStr">
         <is>
           <t>Flexible field for capturing addresses</t>
         </is>
       </c>
-      <c r="G100" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H100" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I100" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3587,17 +3768,18 @@
         </is>
       </c>
       <c r="E101" s="2" t="inlineStr"/>
-      <c r="F101" s="2" t="inlineStr">
+      <c r="F101" s="2" t="inlineStr"/>
+      <c r="G101" s="2" t="inlineStr">
         <is>
           <t>The postal code</t>
         </is>
       </c>
-      <c r="G101" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H101" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I101" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3617,17 +3799,18 @@
         </is>
       </c>
       <c r="E102" s="2" t="inlineStr"/>
-      <c r="F102" s="2" t="inlineStr">
+      <c r="F102" s="2" t="inlineStr"/>
+      <c r="G102" s="2" t="inlineStr">
         <is>
           <t>Easting coordinate in British National Grid (EPSG:27700)</t>
         </is>
       </c>
-      <c r="G102" s="2" t="inlineStr">
+      <c r="H102" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H102" s="2" t="inlineStr">
+      <c r="I102" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3647,17 +3830,18 @@
         </is>
       </c>
       <c r="E103" s="2" t="inlineStr"/>
-      <c r="F103" s="2" t="inlineStr">
+      <c r="F103" s="2" t="inlineStr"/>
+      <c r="G103" s="2" t="inlineStr">
         <is>
           <t>Northing coordinate in British National Grid (EPSG:27700)</t>
         </is>
       </c>
-      <c r="G103" s="2" t="inlineStr">
+      <c r="H103" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H103" s="2" t="inlineStr">
+      <c r="I103" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3677,17 +3861,18 @@
         </is>
       </c>
       <c r="E104" s="2" t="inlineStr"/>
-      <c r="F104" s="2" t="inlineStr">
+      <c r="F104" s="2" t="inlineStr"/>
+      <c r="G104" s="2" t="inlineStr">
         <is>
           <t>Latitude coordinate in WGS84 (EPSG:4326)</t>
         </is>
       </c>
-      <c r="G104" s="2" t="inlineStr">
+      <c r="H104" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H104" s="2" t="inlineStr">
+      <c r="I104" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3707,17 +3892,18 @@
         </is>
       </c>
       <c r="E105" s="2" t="inlineStr"/>
-      <c r="F105" s="2" t="inlineStr">
+      <c r="F105" s="2" t="inlineStr"/>
+      <c r="G105" s="2" t="inlineStr">
         <is>
           <t>Longitude coordinate in WGS84 (EPSG:4326)</t>
         </is>
       </c>
-      <c r="G105" s="2" t="inlineStr">
+      <c r="H105" s="2" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="H105" s="2" t="inlineStr">
+      <c r="I105" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3737,17 +3923,18 @@
         </is>
       </c>
       <c r="E106" s="2" t="inlineStr"/>
-      <c r="F106" s="2" t="inlineStr">
+      <c r="F106" s="2" t="inlineStr"/>
+      <c r="G106" s="2" t="inlineStr">
         <is>
           <t>A text description providing details about the subject. For parking changes, this describes how the proposed works affect existing car parking arrangements.</t>
         </is>
       </c>
-      <c r="G106" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H106" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I106" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3767,17 +3954,18 @@
         </is>
       </c>
       <c r="E107" s="2" t="inlineStr"/>
-      <c r="F107" s="2" t="inlineStr">
+      <c r="F107" s="2" t="inlineStr"/>
+      <c r="G107" s="2" t="inlineStr">
         <is>
           <t>Unique Property Reference Numbers (UPRNs) for properties within the site boundary</t>
         </is>
       </c>
-      <c r="G107" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H107" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I107" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3801,17 +3989,18 @@
       </c>
       <c r="D108" s="2" t="inlineStr"/>
       <c r="E108" s="2" t="inlineStr"/>
-      <c r="F108" s="2" t="inlineStr">
+      <c r="F108" s="2" t="inlineStr"/>
+      <c r="G108" s="2" t="inlineStr">
         <is>
           <t>Can site be seen from a public road, public footpath, bridleway or other public land</t>
         </is>
       </c>
-      <c r="G108" s="2" t="inlineStr">
+      <c r="H108" s="2" t="inlineStr">
         <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="H108" s="2" t="inlineStr">
+      <c r="I108" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -3827,17 +4016,18 @@
       </c>
       <c r="D109" s="2" t="inlineStr"/>
       <c r="E109" s="2" t="inlineStr"/>
-      <c r="F109" s="2" t="inlineStr">
+      <c r="F109" s="2" t="inlineStr"/>
+      <c r="G109" s="2" t="inlineStr">
         <is>
           <t>Indicates who the authority should contact to arrange a site visit</t>
         </is>
       </c>
-      <c r="G109" s="2" t="inlineStr">
+      <c r="H109" s="2" t="inlineStr">
         <is>
           <t>enum</t>
         </is>
       </c>
-      <c r="H109" s="2" t="inlineStr">
+      <c r="I109" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -3853,17 +4043,18 @@
       </c>
       <c r="D110" s="2" t="inlineStr"/>
       <c r="E110" s="2" t="inlineStr"/>
-      <c r="F110" s="2" t="inlineStr">
+      <c r="F110" s="2" t="inlineStr"/>
+      <c r="G110" s="2" t="inlineStr">
         <is>
           <t>The reference of the applicant or agent who should be contacted for site visits</t>
         </is>
       </c>
-      <c r="G110" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H110" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I110" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -3883,17 +4074,18 @@
         </is>
       </c>
       <c r="E111" s="2" t="inlineStr"/>
-      <c r="F111" s="2" t="inlineStr">
+      <c r="F111" s="2" t="inlineStr"/>
+      <c r="G111" s="2" t="inlineStr">
         <is>
           <t>The complete name of a person</t>
         </is>
       </c>
-      <c r="G111" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H111" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I111" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -3913,17 +4105,18 @@
         </is>
       </c>
       <c r="E112" s="2" t="inlineStr"/>
-      <c r="F112" s="2" t="inlineStr">
+      <c r="F112" s="2" t="inlineStr"/>
+      <c r="G112" s="2" t="inlineStr">
         <is>
           <t>A phone number</t>
         </is>
       </c>
-      <c r="G112" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H112" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I112" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -3943,17 +4136,18 @@
         </is>
       </c>
       <c r="E113" s="2" t="inlineStr"/>
-      <c r="F113" s="2" t="inlineStr">
+      <c r="F113" s="2" t="inlineStr"/>
+      <c r="G113" s="2" t="inlineStr">
         <is>
           <t>The email address that can be used for electronic correspondence with the individual</t>
         </is>
       </c>
-      <c r="G113" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
       <c r="H113" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I113" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>

</xml_diff>

<commit_message>
Latest generated outputs 2025-11-12
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/advertising-advertising.xlsx
+++ b/generated/spreadsheet/advertising-advertising.xlsx
@@ -1370,7 +1370,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>date</t>
         </is>
       </c>
       <c r="I27" s="2" t="inlineStr">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="H28" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>date</t>
         </is>
       </c>
       <c r="I28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Latest generated outputs 2025-11-24
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/advertising-advertising.xlsx
+++ b/generated/spreadsheet/advertising-advertising.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2485,17 +2485,17 @@
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>Interest details</t>
+          <t>Interest in land</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>Names and contact details for all parties with an interest in the proposed develpoment.</t>
+          <t>Whether the applicant owns or has permission to use the land where the proposed advertisement will be placed</t>
         </is>
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>Applicant interest</t>
+          <t>Applicant owns land</t>
         </is>
       </c>
       <c r="D61" s="2" t="inlineStr"/>
@@ -2503,12 +2503,12 @@
       <c r="F61" s="2" t="inlineStr"/>
       <c r="G61" s="2" t="inlineStr">
         <is>
-          <t>Description of the applicant's interest in the land</t>
+          <t>True or False indicating whether the applicant owns the land where the advertisement will be displayed</t>
         </is>
       </c>
       <c r="H61" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I61" s="2" t="inlineStr">
@@ -2522,28 +2522,20 @@
       <c r="B62" s="2" t="n"/>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>Owner details[]</t>
-        </is>
-      </c>
-      <c r="D62" s="2" t="inlineStr">
-        <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E62" s="2" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
+          <t>Permission obtained</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr"/>
+      <c r="E62" s="2" t="inlineStr"/>
       <c r="F62" s="2" t="inlineStr"/>
       <c r="G62" s="2" t="inlineStr">
         <is>
-          <t>The title of the individual</t>
+          <t>True or False indicating whether permission of the owner for the display of an advertisement has been obtained</t>
         </is>
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I62" s="2" t="inlineStr">
@@ -2557,23 +2549,15 @@
       <c r="B63" s="2" t="n"/>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>Owner details[]</t>
-        </is>
-      </c>
-      <c r="D63" s="2" t="inlineStr">
-        <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E63" s="2" t="inlineStr">
-        <is>
-          <t>First Name</t>
-        </is>
-      </c>
+          <t>Permission not obtained details</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr"/>
+      <c r="E63" s="2" t="inlineStr"/>
       <c r="F63" s="2" t="inlineStr"/>
       <c r="G63" s="2" t="inlineStr">
         <is>
-          <t>The first name of the individual</t>
+          <t>Details explaining why permission from the land owner has not been obtained for the advertisement display</t>
         </is>
       </c>
       <c r="H63" s="2" t="inlineStr">
@@ -2583,32 +2567,32 @@
       </c>
       <c r="I63" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="n"/>
-      <c r="B64" s="2" t="n"/>
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>Declaration</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>Signed and dated verification of the application's accuracy.</t>
+        </is>
+      </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>Owner details[]</t>
-        </is>
-      </c>
-      <c r="D64" s="2" t="inlineStr">
-        <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E64" s="2" t="inlineStr">
-        <is>
-          <t>Last Name</t>
-        </is>
-      </c>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr"/>
+      <c r="E64" s="2" t="inlineStr"/>
       <c r="F64" s="2" t="inlineStr"/>
       <c r="G64" s="2" t="inlineStr">
         <is>
-          <t>The last name of the individual</t>
+          <t>A name of a person</t>
         </is>
       </c>
       <c r="H64" s="2" t="inlineStr">
@@ -2627,28 +2611,20 @@
       <c r="B65" s="2" t="n"/>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>Owner details[]</t>
-        </is>
-      </c>
-      <c r="D65" s="2" t="inlineStr">
-        <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E65" s="2" t="inlineStr">
-        <is>
-          <t>Address Text</t>
-        </is>
-      </c>
+          <t>Declaration confirmed</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr"/>
+      <c r="E65" s="2" t="inlineStr"/>
       <c r="F65" s="2" t="inlineStr"/>
       <c r="G65" s="2" t="inlineStr">
         <is>
-          <t>Flexible field for capturing addresses</t>
+          <t>Confirms the applicant or agent has reviewed and validated the information provided in the application</t>
         </is>
       </c>
       <c r="H65" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I65" s="2" t="inlineStr">
@@ -2662,23 +2638,15 @@
       <c r="B66" s="2" t="n"/>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>Owner details[]</t>
-        </is>
-      </c>
-      <c r="D66" s="2" t="inlineStr">
-        <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E66" s="2" t="inlineStr">
-        <is>
-          <t>Postcode</t>
-        </is>
-      </c>
+          <t>Declaration date</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr"/>
+      <c r="E66" s="2" t="inlineStr"/>
       <c r="F66" s="2" t="inlineStr"/>
       <c r="G66" s="2" t="inlineStr">
         <is>
-          <t>The postal code</t>
+          <t>The date the declaration was made</t>
         </is>
       </c>
       <c r="H66" s="2" t="inlineStr">
@@ -2688,28 +2656,32 @@
       </c>
       <c r="I66" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="2" t="n"/>
-      <c r="B67" s="2" t="n"/>
+      <c r="A67" s="2" t="inlineStr">
+        <is>
+          <t>Pre-application advice</t>
+        </is>
+      </c>
+      <c r="B67" s="2" t="inlineStr">
+        <is>
+          <t>Details of pre-application advice previously received from the planning authority</t>
+        </is>
+      </c>
       <c r="C67" s="2" t="inlineStr">
         <is>
-          <t>Owner details[]</t>
-        </is>
-      </c>
-      <c r="D67" s="2" t="inlineStr">
-        <is>
-          <t>Informed of application</t>
-        </is>
-      </c>
+          <t>Pre-application advice sought</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="inlineStr"/>
       <c r="E67" s="2" t="inlineStr"/>
       <c r="F67" s="2" t="inlineStr"/>
       <c r="G67" s="2" t="inlineStr">
         <is>
-          <t>Whether the owner has been informed of the application</t>
+          <t>Whether pre-application advice has been sought from the planning authority</t>
         </is>
       </c>
       <c r="H67" s="2" t="inlineStr">
@@ -2728,23 +2700,15 @@
       <c r="B68" s="2" t="n"/>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>Interested persons[]</t>
-        </is>
-      </c>
-      <c r="D68" s="2" t="inlineStr">
-        <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E68" s="2" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
+          <t>Officer name</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr"/>
+      <c r="E68" s="2" t="inlineStr"/>
       <c r="F68" s="2" t="inlineStr"/>
       <c r="G68" s="2" t="inlineStr">
         <is>
-          <t>The title of the individual</t>
+          <t>Name of the planning officer who provided the pre-application advice</t>
         </is>
       </c>
       <c r="H68" s="2" t="inlineStr">
@@ -2763,23 +2727,15 @@
       <c r="B69" s="2" t="n"/>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>Interested persons[]</t>
-        </is>
-      </c>
-      <c r="D69" s="2" t="inlineStr">
-        <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E69" s="2" t="inlineStr">
-        <is>
-          <t>First Name</t>
-        </is>
-      </c>
+          <t>Reference</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="inlineStr"/>
+      <c r="E69" s="2" t="inlineStr"/>
       <c r="F69" s="2" t="inlineStr"/>
       <c r="G69" s="2" t="inlineStr">
         <is>
-          <t>The first name of the individual</t>
+          <t>A unique reference for the data item</t>
         </is>
       </c>
       <c r="H69" s="2" t="inlineStr">
@@ -2789,7 +2745,7 @@
       </c>
       <c r="I69" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -2798,23 +2754,15 @@
       <c r="B70" s="2" t="n"/>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>Interested persons[]</t>
-        </is>
-      </c>
-      <c r="D70" s="2" t="inlineStr">
-        <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E70" s="2" t="inlineStr">
-        <is>
-          <t>Last Name</t>
-        </is>
-      </c>
+          <t>Advice date</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr"/>
+      <c r="E70" s="2" t="inlineStr"/>
       <c r="F70" s="2" t="inlineStr"/>
       <c r="G70" s="2" t="inlineStr">
         <is>
-          <t>The last name of the individual</t>
+          <t>Date when pre-application advice was received, in YYYY-MM-DD format</t>
         </is>
       </c>
       <c r="H70" s="2" t="inlineStr">
@@ -2824,7 +2772,7 @@
       </c>
       <c r="I70" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -2833,23 +2781,15 @@
       <c r="B71" s="2" t="n"/>
       <c r="C71" s="2" t="inlineStr">
         <is>
-          <t>Interested persons[]</t>
-        </is>
-      </c>
-      <c r="D71" s="2" t="inlineStr">
-        <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E71" s="2" t="inlineStr">
-        <is>
-          <t>Address Text</t>
-        </is>
-      </c>
+          <t>Advice summary</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr"/>
+      <c r="E71" s="2" t="inlineStr"/>
       <c r="F71" s="2" t="inlineStr"/>
       <c r="G71" s="2" t="inlineStr">
         <is>
-          <t>Flexible field for capturing addresses</t>
+          <t>Summary of the pre-application advice received from the planning authority</t>
         </is>
       </c>
       <c r="H71" s="2" t="inlineStr">
@@ -2859,37 +2799,41 @@
       </c>
       <c r="I71" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="n"/>
-      <c r="B72" s="2" t="n"/>
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>Proposed advert details</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>Details of the proposed advertisements such as their size and how they are made</t>
+        </is>
+      </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>Interested persons[]</t>
+          <t>Advertisements[]</t>
         </is>
       </c>
       <c r="D72" s="2" t="inlineStr">
         <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E72" s="2" t="inlineStr">
-        <is>
-          <t>Postcode</t>
-        </is>
-      </c>
+          <t>Height from ground</t>
+        </is>
+      </c>
+      <c r="E72" s="2" t="inlineStr"/>
       <c r="F72" s="2" t="inlineStr"/>
       <c r="G72" s="2" t="inlineStr">
         <is>
-          <t>The postal code</t>
+          <t>Height, in metres, from ground to the base of the advertisement</t>
         </is>
       </c>
       <c r="H72" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I72" s="2" t="inlineStr">
@@ -2903,29 +2847,29 @@
       <c r="B73" s="2" t="n"/>
       <c r="C73" s="2" t="inlineStr">
         <is>
-          <t>Interested persons[]</t>
+          <t>Advertisements[]</t>
         </is>
       </c>
       <c r="D73" s="2" t="inlineStr">
         <is>
-          <t>Nature of interest</t>
+          <t>Height</t>
         </is>
       </c>
       <c r="E73" s="2" t="inlineStr"/>
       <c r="F73" s="2" t="inlineStr"/>
       <c r="G73" s="2" t="inlineStr">
         <is>
-          <t>Description of the nature of a person's interest in the property</t>
+          <t>Height, in metres, of dimensions of advertisement</t>
         </is>
       </c>
       <c r="H73" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I73" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -2934,29 +2878,29 @@
       <c r="B74" s="2" t="n"/>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>Interested persons[]</t>
+          <t>Advertisements[]</t>
         </is>
       </c>
       <c r="D74" s="2" t="inlineStr">
         <is>
-          <t>Informed of application</t>
+          <t>Width</t>
         </is>
       </c>
       <c r="E74" s="2" t="inlineStr"/>
       <c r="F74" s="2" t="inlineStr"/>
       <c r="G74" s="2" t="inlineStr">
         <is>
-          <t>Whether the person has been informed of the application</t>
+          <t>Width of dimensions of advertisement</t>
         </is>
       </c>
       <c r="H74" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I74" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -2965,24 +2909,24 @@
       <c r="B75" s="2" t="n"/>
       <c r="C75" s="2" t="inlineStr">
         <is>
-          <t>Interested persons[]</t>
+          <t>Advertisements[]</t>
         </is>
       </c>
       <c r="D75" s="2" t="inlineStr">
         <is>
-          <t>Reason not informed</t>
+          <t>Depth</t>
         </is>
       </c>
       <c r="E75" s="2" t="inlineStr"/>
       <c r="F75" s="2" t="inlineStr"/>
       <c r="G75" s="2" t="inlineStr">
         <is>
-          <t>Reason why a person was not informed of the application</t>
+          <t>Depth, in metres, of dimensions of advertisement</t>
         </is>
       </c>
       <c r="H75" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I75" s="2" t="inlineStr">
@@ -2996,25 +2940,29 @@
       <c r="B76" s="2" t="n"/>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>Applicant owns land</t>
-        </is>
-      </c>
-      <c r="D76" s="2" t="inlineStr"/>
+          <t>Advertisements[]</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>Symbol height max</t>
+        </is>
+      </c>
       <c r="E76" s="2" t="inlineStr"/>
       <c r="F76" s="2" t="inlineStr"/>
       <c r="G76" s="2" t="inlineStr">
         <is>
-          <t>True or False indicating whether the applicant owns the land where the advertisement will be displayed</t>
+          <t>Maximum height, in metres, of any individual letters or symbols</t>
         </is>
       </c>
       <c r="H76" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I76" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -3023,20 +2971,24 @@
       <c r="B77" s="2" t="n"/>
       <c r="C77" s="2" t="inlineStr">
         <is>
-          <t>Permission obtained</t>
-        </is>
-      </c>
-      <c r="D77" s="2" t="inlineStr"/>
+          <t>Advertisements[]</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="inlineStr">
+        <is>
+          <t>Colour</t>
+        </is>
+      </c>
       <c r="E77" s="2" t="inlineStr"/>
       <c r="F77" s="2" t="inlineStr"/>
       <c r="G77" s="2" t="inlineStr">
         <is>
-          <t>True or False indicating whether permission of the owner for the display of an advertisement has been obtained</t>
+          <t>Colour of proposed sign</t>
         </is>
       </c>
       <c r="H77" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I77" s="2" t="inlineStr">
@@ -3050,15 +3002,19 @@
       <c r="B78" s="2" t="n"/>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>Permission not obtained details</t>
-        </is>
-      </c>
-      <c r="D78" s="2" t="inlineStr"/>
+          <t>Advertisements[]</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
       <c r="E78" s="2" t="inlineStr"/>
       <c r="F78" s="2" t="inlineStr"/>
       <c r="G78" s="2" t="inlineStr">
         <is>
-          <t>Details explaining why permission from the land owner has not been obtained for the advertisement display</t>
+          <t>Materials of proposed sign</t>
         </is>
       </c>
       <c r="H78" s="2" t="inlineStr">
@@ -3073,37 +3029,33 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="2" t="inlineStr">
-        <is>
-          <t>Declaration</t>
-        </is>
-      </c>
-      <c r="B79" s="2" t="inlineStr">
-        <is>
-          <t>Signed and dated verification of the application's accuracy.</t>
-        </is>
-      </c>
+      <c r="A79" s="2" t="n"/>
+      <c r="B79" s="2" t="n"/>
       <c r="C79" s="2" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D79" s="2" t="inlineStr"/>
+          <t>Advertisements[]</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>Max projection</t>
+        </is>
+      </c>
       <c r="E79" s="2" t="inlineStr"/>
       <c r="F79" s="2" t="inlineStr"/>
       <c r="G79" s="2" t="inlineStr">
         <is>
-          <t>A name of a person</t>
+          <t>Maximum projection, in metres, of the advertisement from the face of the building</t>
         </is>
       </c>
       <c r="H79" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I79" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -3112,15 +3064,19 @@
       <c r="B80" s="2" t="n"/>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>Declaration confirmed</t>
-        </is>
-      </c>
-      <c r="D80" s="2" t="inlineStr"/>
+          <t>Advertisements[]</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>Illuminated</t>
+        </is>
+      </c>
       <c r="E80" s="2" t="inlineStr"/>
       <c r="F80" s="2" t="inlineStr"/>
       <c r="G80" s="2" t="inlineStr">
         <is>
-          <t>Confirms the applicant or agent has reviewed and validated the information provided in the application</t>
+          <t>Will the sign(s) be illuminated?</t>
         </is>
       </c>
       <c r="H80" s="2" t="inlineStr">
@@ -3130,7 +3086,7 @@
       </c>
       <c r="I80" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -3139,15 +3095,19 @@
       <c r="B81" s="2" t="n"/>
       <c r="C81" s="2" t="inlineStr">
         <is>
-          <t>Declaration date</t>
-        </is>
-      </c>
-      <c r="D81" s="2" t="inlineStr"/>
+          <t>Advertisements[]</t>
+        </is>
+      </c>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>Illumination method</t>
+        </is>
+      </c>
       <c r="E81" s="2" t="inlineStr"/>
       <c r="F81" s="2" t="inlineStr"/>
       <c r="G81" s="2" t="inlineStr">
         <is>
-          <t>The date the declaration was made</t>
+          <t>Method of illumination for the advertisement</t>
         </is>
       </c>
       <c r="H81" s="2" t="inlineStr">
@@ -3157,42 +3117,38 @@
       </c>
       <c r="I81" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="inlineStr">
-        <is>
-          <t>Pre-application advice</t>
-        </is>
-      </c>
-      <c r="B82" s="2" t="inlineStr">
-        <is>
-          <t>Details of pre-application advice previously received from the planning authority</t>
-        </is>
-      </c>
+      <c r="A82" s="2" t="n"/>
+      <c r="B82" s="2" t="n"/>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>Pre-application advice sought</t>
-        </is>
-      </c>
-      <c r="D82" s="2" t="inlineStr"/>
+          <t>Advertisements[]</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>Illuminance level</t>
+        </is>
+      </c>
       <c r="E82" s="2" t="inlineStr"/>
       <c r="F82" s="2" t="inlineStr"/>
       <c r="G82" s="2" t="inlineStr">
         <is>
-          <t>Whether pre-application advice has been sought from the planning authority</t>
+          <t>Level of illuminance for the advertisement</t>
         </is>
       </c>
       <c r="H82" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I82" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -3201,20 +3157,24 @@
       <c r="B83" s="2" t="n"/>
       <c r="C83" s="2" t="inlineStr">
         <is>
-          <t>Officer name</t>
-        </is>
-      </c>
-      <c r="D83" s="2" t="inlineStr"/>
+          <t>Advertisements[]</t>
+        </is>
+      </c>
+      <c r="D83" s="2" t="inlineStr">
+        <is>
+          <t>Illumination type</t>
+        </is>
+      </c>
       <c r="E83" s="2" t="inlineStr"/>
       <c r="F83" s="2" t="inlineStr"/>
       <c r="G83" s="2" t="inlineStr">
         <is>
-          <t>Name of the planning officer who provided the pre-application advice</t>
+          <t>Type of illumination (static or intermittent)</t>
         </is>
       </c>
       <c r="H83" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I83" s="2" t="inlineStr">
@@ -3224,24 +3184,36 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="n"/>
-      <c r="B84" s="2" t="n"/>
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>Site details</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>Where the proposed development will be built.</t>
+        </is>
+      </c>
       <c r="C84" s="2" t="inlineStr">
         <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="D84" s="2" t="inlineStr"/>
+          <t>Site locations[]</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>Site boundary</t>
+        </is>
+      </c>
       <c r="E84" s="2" t="inlineStr"/>
       <c r="F84" s="2" t="inlineStr"/>
       <c r="G84" s="2" t="inlineStr">
         <is>
-          <t>A unique reference for the data item</t>
+          <t>Geometry of the site of the development, typically in GeoJSON format</t>
         </is>
       </c>
       <c r="H84" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>wkt</t>
         </is>
       </c>
       <c r="I84" s="2" t="inlineStr">
@@ -3255,15 +3227,19 @@
       <c r="B85" s="2" t="n"/>
       <c r="C85" s="2" t="inlineStr">
         <is>
-          <t>Advice date</t>
-        </is>
-      </c>
-      <c r="D85" s="2" t="inlineStr"/>
+          <t>Site locations[]</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="inlineStr">
+        <is>
+          <t>Address Text</t>
+        </is>
+      </c>
       <c r="E85" s="2" t="inlineStr"/>
       <c r="F85" s="2" t="inlineStr"/>
       <c r="G85" s="2" t="inlineStr">
         <is>
-          <t>Date when pre-application advice was received, in YYYY-MM-DD format</t>
+          <t>Flexible field for capturing addresses</t>
         </is>
       </c>
       <c r="H85" s="2" t="inlineStr">
@@ -3282,15 +3258,19 @@
       <c r="B86" s="2" t="n"/>
       <c r="C86" s="2" t="inlineStr">
         <is>
-          <t>Advice summary</t>
-        </is>
-      </c>
-      <c r="D86" s="2" t="inlineStr"/>
+          <t>Site locations[]</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>Postcode</t>
+        </is>
+      </c>
       <c r="E86" s="2" t="inlineStr"/>
       <c r="F86" s="2" t="inlineStr"/>
       <c r="G86" s="2" t="inlineStr">
         <is>
-          <t>Summary of the pre-application advice received from the planning authority</t>
+          <t>The postal code</t>
         </is>
       </c>
       <c r="H86" s="2" t="inlineStr">
@@ -3305,31 +3285,23 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="inlineStr">
-        <is>
-          <t>Proposed advert details</t>
-        </is>
-      </c>
-      <c r="B87" s="2" t="inlineStr">
-        <is>
-          <t>Details of the proposed advertisements such as their size and how they are made</t>
-        </is>
-      </c>
+      <c r="A87" s="2" t="n"/>
+      <c r="B87" s="2" t="n"/>
       <c r="C87" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
+          <t>Site locations[]</t>
         </is>
       </c>
       <c r="D87" s="2" t="inlineStr">
         <is>
-          <t>Height from ground</t>
+          <t>Easting</t>
         </is>
       </c>
       <c r="E87" s="2" t="inlineStr"/>
       <c r="F87" s="2" t="inlineStr"/>
       <c r="G87" s="2" t="inlineStr">
         <is>
-          <t>Height, in metres, from ground to the base of the advertisement</t>
+          <t>Easting coordinate in British National Grid (EPSG:27700)</t>
         </is>
       </c>
       <c r="H87" s="2" t="inlineStr">
@@ -3348,19 +3320,19 @@
       <c r="B88" s="2" t="n"/>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
+          <t>Site locations[]</t>
         </is>
       </c>
       <c r="D88" s="2" t="inlineStr">
         <is>
-          <t>Height</t>
+          <t>Northing</t>
         </is>
       </c>
       <c r="E88" s="2" t="inlineStr"/>
       <c r="F88" s="2" t="inlineStr"/>
       <c r="G88" s="2" t="inlineStr">
         <is>
-          <t>Height, in metres, of dimensions of advertisement</t>
+          <t>Northing coordinate in British National Grid (EPSG:27700)</t>
         </is>
       </c>
       <c r="H88" s="2" t="inlineStr">
@@ -3379,19 +3351,19 @@
       <c r="B89" s="2" t="n"/>
       <c r="C89" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
+          <t>Site locations[]</t>
         </is>
       </c>
       <c r="D89" s="2" t="inlineStr">
         <is>
-          <t>Width</t>
+          <t>Latitude</t>
         </is>
       </c>
       <c r="E89" s="2" t="inlineStr"/>
       <c r="F89" s="2" t="inlineStr"/>
       <c r="G89" s="2" t="inlineStr">
         <is>
-          <t>Width of dimensions of advertisement</t>
+          <t>Latitude coordinate in WGS84 (EPSG:4326)</t>
         </is>
       </c>
       <c r="H89" s="2" t="inlineStr">
@@ -3410,19 +3382,19 @@
       <c r="B90" s="2" t="n"/>
       <c r="C90" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
+          <t>Site locations[]</t>
         </is>
       </c>
       <c r="D90" s="2" t="inlineStr">
         <is>
-          <t>Depth</t>
+          <t>Longitude</t>
         </is>
       </c>
       <c r="E90" s="2" t="inlineStr"/>
       <c r="F90" s="2" t="inlineStr"/>
       <c r="G90" s="2" t="inlineStr">
         <is>
-          <t>Depth, in metres, of dimensions of advertisement</t>
+          <t>Longitude coordinate in WGS84 (EPSG:4326)</t>
         </is>
       </c>
       <c r="H90" s="2" t="inlineStr">
@@ -3441,24 +3413,24 @@
       <c r="B91" s="2" t="n"/>
       <c r="C91" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
+          <t>Site locations[]</t>
         </is>
       </c>
       <c r="D91" s="2" t="inlineStr">
         <is>
-          <t>Symbol height max</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="E91" s="2" t="inlineStr"/>
       <c r="F91" s="2" t="inlineStr"/>
       <c r="G91" s="2" t="inlineStr">
         <is>
-          <t>Maximum height, in metres, of any individual letters or symbols</t>
+          <t>A text description providing details about the subject. For parking changes, this describes how the proposed works affect existing car parking arrangements.</t>
         </is>
       </c>
       <c r="H91" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I91" s="2" t="inlineStr">
@@ -3472,19 +3444,19 @@
       <c r="B92" s="2" t="n"/>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
+          <t>Site locations[]</t>
         </is>
       </c>
       <c r="D92" s="2" t="inlineStr">
         <is>
-          <t>Colour</t>
+          <t>UPRNs[]</t>
         </is>
       </c>
       <c r="E92" s="2" t="inlineStr"/>
       <c r="F92" s="2" t="inlineStr"/>
       <c r="G92" s="2" t="inlineStr">
         <is>
-          <t>Colour of proposed sign</t>
+          <t>Unique Property Reference Numbers (UPRNs) for properties within the site boundary</t>
         </is>
       </c>
       <c r="H92" s="2" t="inlineStr">
@@ -3499,33 +3471,37 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="n"/>
-      <c r="B93" s="2" t="n"/>
+      <c r="A93" s="2" t="inlineStr">
+        <is>
+          <t>Site Visit Details</t>
+        </is>
+      </c>
+      <c r="B93" s="2" t="inlineStr">
+        <is>
+          <t>Information to help the planning authority arrange a site visit</t>
+        </is>
+      </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
-        </is>
-      </c>
-      <c r="D93" s="2" t="inlineStr">
-        <is>
-          <t>Materials</t>
-        </is>
-      </c>
+          <t>Site seen from public area</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="inlineStr"/>
       <c r="E93" s="2" t="inlineStr"/>
       <c r="F93" s="2" t="inlineStr"/>
       <c r="G93" s="2" t="inlineStr">
         <is>
-          <t>Materials of proposed sign</t>
+          <t>Can site be seen from a public road, public footpath, bridleway or other public land</t>
         </is>
       </c>
       <c r="H93" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I93" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -3534,29 +3510,25 @@
       <c r="B94" s="2" t="n"/>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
-        </is>
-      </c>
-      <c r="D94" s="2" t="inlineStr">
-        <is>
-          <t>Max projection</t>
-        </is>
-      </c>
+          <t>Site visit contact type</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="inlineStr"/>
       <c r="E94" s="2" t="inlineStr"/>
       <c r="F94" s="2" t="inlineStr"/>
       <c r="G94" s="2" t="inlineStr">
         <is>
-          <t>Maximum projection, in metres, of the advertisement from the face of the building</t>
+          <t>Indicates who the authority should contact to arrange a site visit</t>
         </is>
       </c>
       <c r="H94" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I94" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -3565,24 +3537,20 @@
       <c r="B95" s="2" t="n"/>
       <c r="C95" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
-        </is>
-      </c>
-      <c r="D95" s="2" t="inlineStr">
-        <is>
-          <t>Illuminated</t>
-        </is>
-      </c>
+          <t>Contact reference</t>
+        </is>
+      </c>
+      <c r="D95" s="2" t="inlineStr"/>
       <c r="E95" s="2" t="inlineStr"/>
       <c r="F95" s="2" t="inlineStr"/>
       <c r="G95" s="2" t="inlineStr">
         <is>
-          <t>Will the sign(s) be illuminated?</t>
+          <t>The reference of the applicant or agent who should be contacted for site visits</t>
         </is>
       </c>
       <c r="H95" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I95" s="2" t="inlineStr">
@@ -3596,19 +3564,19 @@
       <c r="B96" s="2" t="n"/>
       <c r="C96" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
+          <t>Other site visit contact</t>
         </is>
       </c>
       <c r="D96" s="2" t="inlineStr">
         <is>
-          <t>Illumination method</t>
+          <t>Full name</t>
         </is>
       </c>
       <c r="E96" s="2" t="inlineStr"/>
       <c r="F96" s="2" t="inlineStr"/>
       <c r="G96" s="2" t="inlineStr">
         <is>
-          <t>Method of illumination for the advertisement</t>
+          <t>The complete name of a person</t>
         </is>
       </c>
       <c r="H96" s="2" t="inlineStr">
@@ -3618,7 +3586,7 @@
       </c>
       <c r="I96" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -3627,29 +3595,29 @@
       <c r="B97" s="2" t="n"/>
       <c r="C97" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
+          <t>Other site visit contact</t>
         </is>
       </c>
       <c r="D97" s="2" t="inlineStr">
         <is>
-          <t>Illuminance level</t>
+          <t>Phone number</t>
         </is>
       </c>
       <c r="E97" s="2" t="inlineStr"/>
       <c r="F97" s="2" t="inlineStr"/>
       <c r="G97" s="2" t="inlineStr">
         <is>
-          <t>Level of illuminance for the advertisement</t>
+          <t>A phone number</t>
         </is>
       </c>
       <c r="H97" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I97" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -3658,496 +3626,27 @@
       <c r="B98" s="2" t="n"/>
       <c r="C98" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
+          <t>Other site visit contact</t>
         </is>
       </c>
       <c r="D98" s="2" t="inlineStr">
         <is>
-          <t>Illumination type</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="E98" s="2" t="inlineStr"/>
       <c r="F98" s="2" t="inlineStr"/>
       <c r="G98" s="2" t="inlineStr">
         <is>
-          <t>Type of illumination (static or intermittent)</t>
+          <t>The email address that can be used for electronic correspondence with the individual</t>
         </is>
       </c>
       <c r="H98" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I98" s="2" t="inlineStr">
-        <is>
-          <t>MAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="2" t="inlineStr">
-        <is>
-          <t>Site details</t>
-        </is>
-      </c>
-      <c r="B99" s="2" t="inlineStr">
-        <is>
-          <t>Where the proposed development will be built.</t>
-        </is>
-      </c>
-      <c r="C99" s="2" t="inlineStr">
-        <is>
-          <t>Site locations[]</t>
-        </is>
-      </c>
-      <c r="D99" s="2" t="inlineStr">
-        <is>
-          <t>Site boundary</t>
-        </is>
-      </c>
-      <c r="E99" s="2" t="inlineStr"/>
-      <c r="F99" s="2" t="inlineStr"/>
-      <c r="G99" s="2" t="inlineStr">
-        <is>
-          <t>Geometry of the site of the development, typically in GeoJSON format</t>
-        </is>
-      </c>
-      <c r="H99" s="2" t="inlineStr">
-        <is>
-          <t>wkt</t>
-        </is>
-      </c>
-      <c r="I99" s="2" t="inlineStr">
-        <is>
-          <t>MAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="2" t="n"/>
-      <c r="B100" s="2" t="n"/>
-      <c r="C100" s="2" t="inlineStr">
-        <is>
-          <t>Site locations[]</t>
-        </is>
-      </c>
-      <c r="D100" s="2" t="inlineStr">
-        <is>
-          <t>Address Text</t>
-        </is>
-      </c>
-      <c r="E100" s="2" t="inlineStr"/>
-      <c r="F100" s="2" t="inlineStr"/>
-      <c r="G100" s="2" t="inlineStr">
-        <is>
-          <t>Flexible field for capturing addresses</t>
-        </is>
-      </c>
-      <c r="H100" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I100" s="2" t="inlineStr">
-        <is>
-          <t>MAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="2" t="n"/>
-      <c r="B101" s="2" t="n"/>
-      <c r="C101" s="2" t="inlineStr">
-        <is>
-          <t>Site locations[]</t>
-        </is>
-      </c>
-      <c r="D101" s="2" t="inlineStr">
-        <is>
-          <t>Postcode</t>
-        </is>
-      </c>
-      <c r="E101" s="2" t="inlineStr"/>
-      <c r="F101" s="2" t="inlineStr"/>
-      <c r="G101" s="2" t="inlineStr">
-        <is>
-          <t>The postal code</t>
-        </is>
-      </c>
-      <c r="H101" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I101" s="2" t="inlineStr">
-        <is>
-          <t>MAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="2" t="n"/>
-      <c r="B102" s="2" t="n"/>
-      <c r="C102" s="2" t="inlineStr">
-        <is>
-          <t>Site locations[]</t>
-        </is>
-      </c>
-      <c r="D102" s="2" t="inlineStr">
-        <is>
-          <t>Easting</t>
-        </is>
-      </c>
-      <c r="E102" s="2" t="inlineStr"/>
-      <c r="F102" s="2" t="inlineStr"/>
-      <c r="G102" s="2" t="inlineStr">
-        <is>
-          <t>Easting coordinate in British National Grid (EPSG:27700)</t>
-        </is>
-      </c>
-      <c r="H102" s="2" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="I102" s="2" t="inlineStr">
-        <is>
-          <t>MAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="2" t="n"/>
-      <c r="B103" s="2" t="n"/>
-      <c r="C103" s="2" t="inlineStr">
-        <is>
-          <t>Site locations[]</t>
-        </is>
-      </c>
-      <c r="D103" s="2" t="inlineStr">
-        <is>
-          <t>Northing</t>
-        </is>
-      </c>
-      <c r="E103" s="2" t="inlineStr"/>
-      <c r="F103" s="2" t="inlineStr"/>
-      <c r="G103" s="2" t="inlineStr">
-        <is>
-          <t>Northing coordinate in British National Grid (EPSG:27700)</t>
-        </is>
-      </c>
-      <c r="H103" s="2" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="I103" s="2" t="inlineStr">
-        <is>
-          <t>MAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="2" t="n"/>
-      <c r="B104" s="2" t="n"/>
-      <c r="C104" s="2" t="inlineStr">
-        <is>
-          <t>Site locations[]</t>
-        </is>
-      </c>
-      <c r="D104" s="2" t="inlineStr">
-        <is>
-          <t>Latitude</t>
-        </is>
-      </c>
-      <c r="E104" s="2" t="inlineStr"/>
-      <c r="F104" s="2" t="inlineStr"/>
-      <c r="G104" s="2" t="inlineStr">
-        <is>
-          <t>Latitude coordinate in WGS84 (EPSG:4326)</t>
-        </is>
-      </c>
-      <c r="H104" s="2" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="I104" s="2" t="inlineStr">
-        <is>
-          <t>MAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="2" t="n"/>
-      <c r="B105" s="2" t="n"/>
-      <c r="C105" s="2" t="inlineStr">
-        <is>
-          <t>Site locations[]</t>
-        </is>
-      </c>
-      <c r="D105" s="2" t="inlineStr">
-        <is>
-          <t>Longitude</t>
-        </is>
-      </c>
-      <c r="E105" s="2" t="inlineStr"/>
-      <c r="F105" s="2" t="inlineStr"/>
-      <c r="G105" s="2" t="inlineStr">
-        <is>
-          <t>Longitude coordinate in WGS84 (EPSG:4326)</t>
-        </is>
-      </c>
-      <c r="H105" s="2" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="I105" s="2" t="inlineStr">
-        <is>
-          <t>MAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="2" t="n"/>
-      <c r="B106" s="2" t="n"/>
-      <c r="C106" s="2" t="inlineStr">
-        <is>
-          <t>Site locations[]</t>
-        </is>
-      </c>
-      <c r="D106" s="2" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="E106" s="2" t="inlineStr"/>
-      <c r="F106" s="2" t="inlineStr"/>
-      <c r="G106" s="2" t="inlineStr">
-        <is>
-          <t>A text description providing details about the subject. For parking changes, this describes how the proposed works affect existing car parking arrangements.</t>
-        </is>
-      </c>
-      <c r="H106" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I106" s="2" t="inlineStr">
-        <is>
-          <t>MAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="2" t="n"/>
-      <c r="B107" s="2" t="n"/>
-      <c r="C107" s="2" t="inlineStr">
-        <is>
-          <t>Site locations[]</t>
-        </is>
-      </c>
-      <c r="D107" s="2" t="inlineStr">
-        <is>
-          <t>UPRNs[]</t>
-        </is>
-      </c>
-      <c r="E107" s="2" t="inlineStr"/>
-      <c r="F107" s="2" t="inlineStr"/>
-      <c r="G107" s="2" t="inlineStr">
-        <is>
-          <t>Unique Property Reference Numbers (UPRNs) for properties within the site boundary</t>
-        </is>
-      </c>
-      <c r="H107" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I107" s="2" t="inlineStr">
-        <is>
-          <t>MAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="2" t="inlineStr">
-        <is>
-          <t>Site Visit Details</t>
-        </is>
-      </c>
-      <c r="B108" s="2" t="inlineStr">
-        <is>
-          <t>Information to help the planning authority arrange a site visit</t>
-        </is>
-      </c>
-      <c r="C108" s="2" t="inlineStr">
-        <is>
-          <t>Site seen from public area</t>
-        </is>
-      </c>
-      <c r="D108" s="2" t="inlineStr"/>
-      <c r="E108" s="2" t="inlineStr"/>
-      <c r="F108" s="2" t="inlineStr"/>
-      <c r="G108" s="2" t="inlineStr">
-        <is>
-          <t>Can site be seen from a public road, public footpath, bridleway or other public land</t>
-        </is>
-      </c>
-      <c r="H108" s="2" t="inlineStr">
-        <is>
-          <t>boolean</t>
-        </is>
-      </c>
-      <c r="I108" s="2" t="inlineStr">
-        <is>
-          <t>MUST</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="2" t="n"/>
-      <c r="B109" s="2" t="n"/>
-      <c r="C109" s="2" t="inlineStr">
-        <is>
-          <t>Site visit contact type</t>
-        </is>
-      </c>
-      <c r="D109" s="2" t="inlineStr"/>
-      <c r="E109" s="2" t="inlineStr"/>
-      <c r="F109" s="2" t="inlineStr"/>
-      <c r="G109" s="2" t="inlineStr">
-        <is>
-          <t>Indicates who the authority should contact to arrange a site visit</t>
-        </is>
-      </c>
-      <c r="H109" s="2" t="inlineStr">
-        <is>
-          <t>enum</t>
-        </is>
-      </c>
-      <c r="I109" s="2" t="inlineStr">
-        <is>
-          <t>MUST</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="2" t="n"/>
-      <c r="B110" s="2" t="n"/>
-      <c r="C110" s="2" t="inlineStr">
-        <is>
-          <t>Contact reference</t>
-        </is>
-      </c>
-      <c r="D110" s="2" t="inlineStr"/>
-      <c r="E110" s="2" t="inlineStr"/>
-      <c r="F110" s="2" t="inlineStr"/>
-      <c r="G110" s="2" t="inlineStr">
-        <is>
-          <t>The reference of the applicant or agent who should be contacted for site visits</t>
-        </is>
-      </c>
-      <c r="H110" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I110" s="2" t="inlineStr">
-        <is>
-          <t>MAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="2" t="n"/>
-      <c r="B111" s="2" t="n"/>
-      <c r="C111" s="2" t="inlineStr">
-        <is>
-          <t>Other site visit contact</t>
-        </is>
-      </c>
-      <c r="D111" s="2" t="inlineStr">
-        <is>
-          <t>Full name</t>
-        </is>
-      </c>
-      <c r="E111" s="2" t="inlineStr"/>
-      <c r="F111" s="2" t="inlineStr"/>
-      <c r="G111" s="2" t="inlineStr">
-        <is>
-          <t>The complete name of a person</t>
-        </is>
-      </c>
-      <c r="H111" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I111" s="2" t="inlineStr">
-        <is>
-          <t>MUST</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="2" t="n"/>
-      <c r="B112" s="2" t="n"/>
-      <c r="C112" s="2" t="inlineStr">
-        <is>
-          <t>Other site visit contact</t>
-        </is>
-      </c>
-      <c r="D112" s="2" t="inlineStr">
-        <is>
-          <t>Phone number</t>
-        </is>
-      </c>
-      <c r="E112" s="2" t="inlineStr"/>
-      <c r="F112" s="2" t="inlineStr"/>
-      <c r="G112" s="2" t="inlineStr">
-        <is>
-          <t>A phone number</t>
-        </is>
-      </c>
-      <c r="H112" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I112" s="2" t="inlineStr">
-        <is>
-          <t>MUST</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="2" t="n"/>
-      <c r="B113" s="2" t="n"/>
-      <c r="C113" s="2" t="inlineStr">
-        <is>
-          <t>Other site visit contact</t>
-        </is>
-      </c>
-      <c r="D113" s="2" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="E113" s="2" t="inlineStr"/>
-      <c r="F113" s="2" t="inlineStr"/>
-      <c r="G113" s="2" t="inlineStr">
-        <is>
-          <t>The email address that can be used for electronic correspondence with the individual</t>
-        </is>
-      </c>
-      <c r="H113" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I113" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -4156,39 +3655,39 @@
   </sheetData>
   <mergeCells count="34">
     <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B87:B98"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="A99:A107"/>
     <mergeCell ref="B55"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B93:B98"/>
+    <mergeCell ref="B84:B92"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A58:A60"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B99:B107"/>
-    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="A64:A66"/>
     <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B79:B81"/>
     <mergeCell ref="B2:B20"/>
-    <mergeCell ref="A108:A113"/>
+    <mergeCell ref="B72:B83"/>
     <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A67:A71"/>
     <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A87:A98"/>
-    <mergeCell ref="A82:A86"/>
     <mergeCell ref="A37:A44"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A61:A63"/>
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="B37:B44"/>
-    <mergeCell ref="A61:A78"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B67:B71"/>
     <mergeCell ref="A2:A20"/>
     <mergeCell ref="A55"/>
-    <mergeCell ref="B108:B113"/>
-    <mergeCell ref="B61:B78"/>
     <mergeCell ref="B56:B57"/>
     <mergeCell ref="B49:B54"/>
     <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A72:A83"/>
+    <mergeCell ref="A93:A98"/>
+    <mergeCell ref="A84:A92"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest generated outputs 2025-12-19
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/advertising-advertising.xlsx
+++ b/generated/spreadsheet/advertising-advertising.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -847,12 +847,12 @@
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>URL</t>
+          <t>Base64</t>
         </is>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>A URL pointing to the stored file</t>
+          <t>Base64-encoded content of the file for inline file uploads</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
@@ -886,12 +886,12 @@
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>Base64</t>
+          <t>Filename</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Base64-encoded content of the file for inline file uploads</t>
+          <t>Name of the file being uploaded</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="I13" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -925,12 +925,12 @@
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>Filename</t>
+          <t>MIME type</t>
         </is>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>Name of the file being uploaded</t>
+          <t>The file's MIME type such as application/pdf or image/jpeg</t>
         </is>
       </c>
       <c r="H14" s="2" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="I14" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -964,12 +964,12 @@
       </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>MIME type</t>
+          <t>Checksum</t>
         </is>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>The file's MIME type such as application/pdf or image/jpeg</t>
+          <t>Hash of the file contents used for file validation and checking files have not been tampered with</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1003,17 +1003,17 @@
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>Checksum</t>
+          <t>File size</t>
         </is>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>Hash of the file contents used for file validation and checking files have not been tampered with</t>
+          <t>Size of the file in bytes that can be used to enforce limits</t>
         </is>
       </c>
       <c r="H16" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I16" s="2" t="inlineStr">
@@ -1032,22 +1032,18 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>Documents[]</t>
+          <t>Fee</t>
         </is>
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>File</t>
-        </is>
-      </c>
-      <c r="F17" s="2" t="inlineStr">
-        <is>
-          <t>File size</t>
-        </is>
-      </c>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr"/>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>Size of the file in bytes that can be used to enforce limits</t>
+          <t>The total amount due for the application fee</t>
         </is>
       </c>
       <c r="H17" s="2" t="inlineStr">
@@ -1057,7 +1053,7 @@
       </c>
       <c r="I17" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -1076,13 +1072,13 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Amount</t>
+          <t>Amount paid</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr"/>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>The total amount due for the application fee</t>
+          <t>The amount paid towards the application fee</t>
         </is>
       </c>
       <c r="H18" s="2" t="inlineStr">
@@ -1111,75 +1107,67 @@
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>Amount paid</t>
+          <t>Transactions[]</t>
         </is>
       </c>
       <c r="F19" s="2" t="inlineStr"/>
       <c r="G19" s="2" t="inlineStr">
         <is>
-          <t>The amount paid towards the application fee</t>
+          <t>References to payments or financial transactions related to this application</t>
         </is>
       </c>
       <c r="H19" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I19" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n"/>
-      <c r="B20" s="2" t="n"/>
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>Advertisement location</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>Where the advertisement being applied to be built will be located</t>
+        </is>
+      </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Application</t>
-        </is>
-      </c>
-      <c r="D20" s="2" t="inlineStr">
-        <is>
-          <t>Fee</t>
-        </is>
-      </c>
-      <c r="E20" s="2" t="inlineStr">
-        <is>
-          <t>Transactions[]</t>
-        </is>
-      </c>
+          <t>Is advert in place</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr"/>
+      <c r="E20" s="2" t="inlineStr"/>
       <c r="F20" s="2" t="inlineStr"/>
       <c r="G20" s="2" t="inlineStr">
         <is>
-          <t>References to payments or financial transactions related to this application</t>
+          <t>Whether the advertisement is already in place</t>
         </is>
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I20" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>Advertisement location</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>Where the advertisement being applied to be built will be located</t>
-        </is>
-      </c>
+      <c r="A21" s="2" t="n"/>
+      <c r="B21" s="2" t="n"/>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Is advert in place</t>
+          <t>Advert placed date</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr"/>
@@ -1187,17 +1175,17 @@
       <c r="F21" s="2" t="inlineStr"/>
       <c r="G21" s="2" t="inlineStr">
         <is>
-          <t>Whether the advertisement is already in place</t>
+          <t>Date when the advertisement was placed (YYYY-MM-DD format)</t>
         </is>
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>date</t>
         </is>
       </c>
       <c r="I21" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1194,7 @@
       <c r="B22" s="2" t="n"/>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Advert placed date</t>
+          <t>Is replacement advert</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr"/>
@@ -1214,17 +1202,17 @@
       <c r="F22" s="2" t="inlineStr"/>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>Date when the advertisement was placed (YYYY-MM-DD format)</t>
+          <t>Whether this is a replacement advertisement</t>
         </is>
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I22" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -1233,20 +1221,24 @@
       <c r="B23" s="2" t="n"/>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>Is replacement advert</t>
-        </is>
-      </c>
-      <c r="D23" s="2" t="inlineStr"/>
+          <t>Document reference[]</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>Reference</t>
+        </is>
+      </c>
       <c r="E23" s="2" t="inlineStr"/>
       <c r="F23" s="2" t="inlineStr"/>
       <c r="G23" s="2" t="inlineStr">
         <is>
-          <t>Whether this is a replacement advertisement</t>
+          <t>A unique reference for the data item</t>
         </is>
       </c>
       <c r="H23" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I23" s="2" t="inlineStr">
@@ -1265,14 +1257,14 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>Reference</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr"/>
       <c r="F24" s="2" t="inlineStr"/>
       <c r="G24" s="2" t="inlineStr">
         <is>
-          <t>A unique reference for the data item</t>
+          <t>A name for the document. For example, The Site Plan</t>
         </is>
       </c>
       <c r="H24" s="2" t="inlineStr">
@@ -1291,24 +1283,20 @@
       <c r="B25" s="2" t="n"/>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>Document reference[]</t>
-        </is>
-      </c>
-      <c r="D25" s="2" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
+          <t>Is advert overhanging</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr"/>
       <c r="E25" s="2" t="inlineStr"/>
       <c r="F25" s="2" t="inlineStr"/>
       <c r="G25" s="2" t="inlineStr">
         <is>
-          <t>A name for the document. For example, The Site Plan</t>
+          <t>Whether the advertisement will project over a footpath or other public highway</t>
         </is>
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I25" s="2" t="inlineStr">
@@ -1318,11 +1306,19 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n"/>
-      <c r="B26" s="2" t="n"/>
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>Advert period</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>How long the proposed advertisement will be shown.</t>
+        </is>
+      </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>Is advert overhanging</t>
+          <t>Advert start date</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr"/>
@@ -1330,12 +1326,12 @@
       <c r="F26" s="2" t="inlineStr"/>
       <c r="G26" s="2" t="inlineStr">
         <is>
-          <t>Whether the advertisement will project over a footpath or other public highway</t>
+          <t>The start of the time period that consent to advertisement is sought</t>
         </is>
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>date</t>
         </is>
       </c>
       <c r="I26" s="2" t="inlineStr">
@@ -1345,19 +1341,11 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>Advert period</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="inlineStr">
-        <is>
-          <t>How long the proposed advertisement will be shown.</t>
-        </is>
-      </c>
+      <c r="A27" s="2" t="n"/>
+      <c r="B27" s="2" t="n"/>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>Advert start date</t>
+          <t>Advert end date</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr"/>
@@ -1365,7 +1353,7 @@
       <c r="F27" s="2" t="inlineStr"/>
       <c r="G27" s="2" t="inlineStr">
         <is>
-          <t>The start of the time period that consent to advertisement is sought</t>
+          <t>The end of the time period that consent to advertisement is sought</t>
         </is>
       </c>
       <c r="H27" s="2" t="inlineStr">
@@ -1380,11 +1368,19 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="n"/>
-      <c r="B28" s="2" t="n"/>
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>Advertisement types</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>What type of advertisements are proposed and how many there will be.</t>
+        </is>
+      </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>Advert end date</t>
+          <t>Advertisement proposal description</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr"/>
@@ -1392,12 +1388,12 @@
       <c r="F28" s="2" t="inlineStr"/>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>The end of the time period that consent to advertisement is sought</t>
+          <t>Description of the advertisement proposal</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I28" s="2" t="inlineStr">
@@ -1407,32 +1403,28 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>Advertisement types</t>
-        </is>
-      </c>
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>What type of advertisements are proposed and how many there will be.</t>
-        </is>
-      </c>
+      <c r="A29" s="2" t="n"/>
+      <c r="B29" s="2" t="n"/>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>Advertisement proposal description</t>
-        </is>
-      </c>
-      <c r="D29" s="2" t="inlineStr"/>
+          <t>Advertisement proposal type[]</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>Advertisement type</t>
+        </is>
+      </c>
       <c r="E29" s="2" t="inlineStr"/>
       <c r="F29" s="2" t="inlineStr"/>
       <c r="G29" s="2" t="inlineStr">
         <is>
-          <t>Description of the advertisement proposal</t>
+          <t>One of the advertisement-types or other</t>
         </is>
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I29" s="2" t="inlineStr">
@@ -1451,19 +1443,19 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>Advertisement type</t>
+          <t>Advertisement count</t>
         </is>
       </c>
       <c r="E30" s="2" t="inlineStr"/>
       <c r="F30" s="2" t="inlineStr"/>
       <c r="G30" s="2" t="inlineStr">
         <is>
-          <t>One of the advertisement-types or other</t>
+          <t>Number of this type of advertisement</t>
         </is>
       </c>
       <c r="H30" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I30" s="2" t="inlineStr">
@@ -1482,45 +1474,49 @@
       </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>Advertisement count</t>
+          <t>Advertisement other description</t>
         </is>
       </c>
       <c r="E31" s="2" t="inlineStr"/>
       <c r="F31" s="2" t="inlineStr"/>
       <c r="G31" s="2" t="inlineStr">
         <is>
-          <t>Number of this type of advertisement</t>
+          <t>Details required if other advertisement type is selected</t>
         </is>
       </c>
       <c r="H31" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I31" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="n"/>
-      <c r="B32" s="2" t="n"/>
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Agent contact details</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>Name and contact information if an agent is being used.</t>
+        </is>
+      </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>Advertisement proposal type[]</t>
-        </is>
-      </c>
-      <c r="D32" s="2" t="inlineStr">
-        <is>
-          <t>Advertisement other description</t>
-        </is>
-      </c>
+          <t>Agent reference</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr"/>
       <c r="E32" s="2" t="inlineStr"/>
       <c r="F32" s="2" t="inlineStr"/>
       <c r="G32" s="2" t="inlineStr">
         <is>
-          <t>Details required if other advertisement type is selected</t>
+          <t>A reference to an agent object</t>
         </is>
       </c>
       <c r="H32" s="2" t="inlineStr">
@@ -1530,32 +1526,28 @@
       </c>
       <c r="I32" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>Agent contact details</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="inlineStr">
-        <is>
-          <t>Name and contact information if an agent is being used.</t>
-        </is>
-      </c>
+      <c r="A33" s="2" t="n"/>
+      <c r="B33" s="2" t="n"/>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>Agent reference</t>
-        </is>
-      </c>
-      <c r="D33" s="2" t="inlineStr"/>
+          <t>Contact details</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
       <c r="E33" s="2" t="inlineStr"/>
       <c r="F33" s="2" t="inlineStr"/>
       <c r="G33" s="2" t="inlineStr">
         <is>
-          <t>A reference to an agent object</t>
+          <t>The email address that can be used for electronic correspondence with the individual</t>
         </is>
       </c>
       <c r="H33" s="2" t="inlineStr">
@@ -1579,14 +1571,18 @@
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="E34" s="2" t="inlineStr"/>
+          <t>Phone number(s)[]</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>Phone number</t>
+        </is>
+      </c>
       <c r="F34" s="2" t="inlineStr"/>
       <c r="G34" s="2" t="inlineStr">
         <is>
-          <t>The email address that can be used for electronic correspondence with the individual</t>
+          <t>A phone number</t>
         </is>
       </c>
       <c r="H34" s="2" t="inlineStr">
@@ -1596,7 +1592,7 @@
       </c>
       <c r="I34" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -1615,18 +1611,18 @@
       </c>
       <c r="E35" s="2" t="inlineStr">
         <is>
-          <t>Phone number</t>
+          <t>Contact priority</t>
         </is>
       </c>
       <c r="F35" s="2" t="inlineStr"/>
       <c r="G35" s="2" t="inlineStr">
         <is>
-          <t>A phone number</t>
+          <t>The priority of a number</t>
         </is>
       </c>
       <c r="H35" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I35" s="2" t="inlineStr">
@@ -1636,51 +1632,47 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="n"/>
-      <c r="B36" s="2" t="n"/>
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>Agent details</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>Name and contact information if an agent is being used.</t>
+        </is>
+      </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>Contact details</t>
+          <t>agent</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
         <is>
-          <t>Phone number(s)[]</t>
-        </is>
-      </c>
-      <c r="E36" s="2" t="inlineStr">
-        <is>
-          <t>Contact priority</t>
-        </is>
-      </c>
+          <t>Reference</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr"/>
       <c r="F36" s="2" t="inlineStr"/>
       <c r="G36" s="2" t="inlineStr">
         <is>
-          <t>The priority of a number</t>
+          <t>A unique reference for the data item</t>
         </is>
       </c>
       <c r="H36" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I36" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="inlineStr">
-        <is>
-          <t>Agent details</t>
-        </is>
-      </c>
-      <c r="B37" s="2" t="inlineStr">
-        <is>
-          <t>Name and contact information if an agent is being used.</t>
-        </is>
-      </c>
+      <c r="A37" s="2" t="n"/>
+      <c r="B37" s="2" t="n"/>
       <c r="C37" s="2" t="inlineStr">
         <is>
           <t>agent</t>
@@ -1688,14 +1680,18 @@
       </c>
       <c r="D37" s="2" t="inlineStr">
         <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="E37" s="2" t="inlineStr"/>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
       <c r="F37" s="2" t="inlineStr"/>
       <c r="G37" s="2" t="inlineStr">
         <is>
-          <t>A unique reference for the data item</t>
+          <t>The title of the individual</t>
         </is>
       </c>
       <c r="H37" s="2" t="inlineStr">
@@ -1705,7 +1701,7 @@
       </c>
       <c r="I37" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -1724,13 +1720,13 @@
       </c>
       <c r="E38" s="2" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>First Name</t>
         </is>
       </c>
       <c r="F38" s="2" t="inlineStr"/>
       <c r="G38" s="2" t="inlineStr">
         <is>
-          <t>The title of the individual</t>
+          <t>The first name of the individual</t>
         </is>
       </c>
       <c r="H38" s="2" t="inlineStr">
@@ -1740,7 +1736,7 @@
       </c>
       <c r="I38" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -1759,13 +1755,13 @@
       </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>Last Name</t>
         </is>
       </c>
       <c r="F39" s="2" t="inlineStr"/>
       <c r="G39" s="2" t="inlineStr">
         <is>
-          <t>The first name of the individual</t>
+          <t>The last name of the individual</t>
         </is>
       </c>
       <c r="H39" s="2" t="inlineStr">
@@ -1794,13 +1790,13 @@
       </c>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>Address Text</t>
         </is>
       </c>
       <c r="F40" s="2" t="inlineStr"/>
       <c r="G40" s="2" t="inlineStr">
         <is>
-          <t>The last name of the individual</t>
+          <t>Flexible field for capturing addresses</t>
         </is>
       </c>
       <c r="H40" s="2" t="inlineStr">
@@ -1829,13 +1825,13 @@
       </c>
       <c r="E41" s="2" t="inlineStr">
         <is>
-          <t>Address Text</t>
+          <t>Postcode</t>
         </is>
       </c>
       <c r="F41" s="2" t="inlineStr"/>
       <c r="G41" s="2" t="inlineStr">
         <is>
-          <t>Flexible field for capturing addresses</t>
+          <t>The postal code</t>
         </is>
       </c>
       <c r="H41" s="2" t="inlineStr">
@@ -1845,7 +1841,7 @@
       </c>
       <c r="I41" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -1859,18 +1855,14 @@
       </c>
       <c r="D42" s="2" t="inlineStr">
         <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E42" s="2" t="inlineStr">
-        <is>
-          <t>Postcode</t>
-        </is>
-      </c>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr"/>
       <c r="F42" s="2" t="inlineStr"/>
       <c r="G42" s="2" t="inlineStr">
         <is>
-          <t>The postal code</t>
+          <t>The name of a company (that the agent works for)</t>
         </is>
       </c>
       <c r="H42" s="2" t="inlineStr">
@@ -1894,19 +1886,19 @@
       </c>
       <c r="D43" s="2" t="inlineStr">
         <is>
-          <t>Company</t>
+          <t>User role</t>
         </is>
       </c>
       <c r="E43" s="2" t="inlineStr"/>
       <c r="F43" s="2" t="inlineStr"/>
       <c r="G43" s="2" t="inlineStr">
         <is>
-          <t>The name of a company (that the agent works for)</t>
+          <t>The role of the named individual. Agent or proxy</t>
         </is>
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I43" s="2" t="inlineStr">
@@ -1916,58 +1908,58 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="n"/>
-      <c r="B44" s="2" t="n"/>
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>Applicant contact details</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="inlineStr">
+        <is>
+          <t>Telephone number and email address of the applicant.</t>
+        </is>
+      </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>agent</t>
-        </is>
-      </c>
-      <c r="D44" s="2" t="inlineStr">
-        <is>
-          <t>User role</t>
-        </is>
-      </c>
+          <t>Applicant reference</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr"/>
       <c r="E44" s="2" t="inlineStr"/>
       <c r="F44" s="2" t="inlineStr"/>
       <c r="G44" s="2" t="inlineStr">
         <is>
-          <t>The role of the named individual. Agent or proxy</t>
+          <t>Reference to match contact details to a named individual from the applicant details component</t>
         </is>
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I44" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="inlineStr">
-        <is>
-          <t>Applicant contact details</t>
-        </is>
-      </c>
-      <c r="B45" s="2" t="inlineStr">
-        <is>
-          <t>Telephone number and email address of the applicant.</t>
-        </is>
-      </c>
+      <c r="A45" s="2" t="n"/>
+      <c r="B45" s="2" t="n"/>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>Applicant reference</t>
-        </is>
-      </c>
-      <c r="D45" s="2" t="inlineStr"/>
+          <t>Contact details</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
       <c r="E45" s="2" t="inlineStr"/>
       <c r="F45" s="2" t="inlineStr"/>
       <c r="G45" s="2" t="inlineStr">
         <is>
-          <t>Reference to match contact details to a named individual from the applicant details component</t>
+          <t>The email address that can be used for electronic correspondence with the individual</t>
         </is>
       </c>
       <c r="H45" s="2" t="inlineStr">
@@ -1991,14 +1983,18 @@
       </c>
       <c r="D46" s="2" t="inlineStr">
         <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="E46" s="2" t="inlineStr"/>
+          <t>Phone number(s)[]</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>Phone number</t>
+        </is>
+      </c>
       <c r="F46" s="2" t="inlineStr"/>
       <c r="G46" s="2" t="inlineStr">
         <is>
-          <t>The email address that can be used for electronic correspondence with the individual</t>
+          <t>A phone number</t>
         </is>
       </c>
       <c r="H46" s="2" t="inlineStr">
@@ -2008,7 +2004,7 @@
       </c>
       <c r="I46" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -2027,18 +2023,18 @@
       </c>
       <c r="E47" s="2" t="inlineStr">
         <is>
-          <t>Phone number</t>
+          <t>Contact priority</t>
         </is>
       </c>
       <c r="F47" s="2" t="inlineStr"/>
       <c r="G47" s="2" t="inlineStr">
         <is>
-          <t>A phone number</t>
+          <t>The priority of a number</t>
         </is>
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I47" s="2" t="inlineStr">
@@ -2048,51 +2044,47 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="n"/>
-      <c r="B48" s="2" t="n"/>
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>Applicant details</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>Name and contact information for the parties making the application.</t>
+        </is>
+      </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>Contact details</t>
+          <t>Applicants[]</t>
         </is>
       </c>
       <c r="D48" s="2" t="inlineStr">
         <is>
-          <t>Phone number(s)[]</t>
-        </is>
-      </c>
-      <c r="E48" s="2" t="inlineStr">
-        <is>
-          <t>Contact priority</t>
-        </is>
-      </c>
+          <t>Reference</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr"/>
       <c r="F48" s="2" t="inlineStr"/>
       <c r="G48" s="2" t="inlineStr">
         <is>
-          <t>The priority of a number</t>
+          <t>A unique reference for the data item</t>
         </is>
       </c>
       <c r="H48" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I48" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="inlineStr">
-        <is>
-          <t>Applicant details</t>
-        </is>
-      </c>
-      <c r="B49" s="2" t="inlineStr">
-        <is>
-          <t>Name and contact information for the parties making the application.</t>
-        </is>
-      </c>
+      <c r="A49" s="2" t="n"/>
+      <c r="B49" s="2" t="n"/>
       <c r="C49" s="2" t="inlineStr">
         <is>
           <t>Applicants[]</t>
@@ -2100,14 +2092,18 @@
       </c>
       <c r="D49" s="2" t="inlineStr">
         <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="E49" s="2" t="inlineStr"/>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
       <c r="F49" s="2" t="inlineStr"/>
       <c r="G49" s="2" t="inlineStr">
         <is>
-          <t>A unique reference for the data item</t>
+          <t>The title of the individual</t>
         </is>
       </c>
       <c r="H49" s="2" t="inlineStr">
@@ -2117,7 +2113,7 @@
       </c>
       <c r="I49" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -2136,13 +2132,13 @@
       </c>
       <c r="E50" s="2" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>First Name</t>
         </is>
       </c>
       <c r="F50" s="2" t="inlineStr"/>
       <c r="G50" s="2" t="inlineStr">
         <is>
-          <t>The title of the individual</t>
+          <t>The first name of the individual</t>
         </is>
       </c>
       <c r="H50" s="2" t="inlineStr">
@@ -2152,7 +2148,7 @@
       </c>
       <c r="I50" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -2171,13 +2167,13 @@
       </c>
       <c r="E51" s="2" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>Last Name</t>
         </is>
       </c>
       <c r="F51" s="2" t="inlineStr"/>
       <c r="G51" s="2" t="inlineStr">
         <is>
-          <t>The first name of the individual</t>
+          <t>The last name of the individual</t>
         </is>
       </c>
       <c r="H51" s="2" t="inlineStr">
@@ -2206,13 +2202,13 @@
       </c>
       <c r="E52" s="2" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>Address Text</t>
         </is>
       </c>
       <c r="F52" s="2" t="inlineStr"/>
       <c r="G52" s="2" t="inlineStr">
         <is>
-          <t>The last name of the individual</t>
+          <t>Flexible field for capturing addresses</t>
         </is>
       </c>
       <c r="H52" s="2" t="inlineStr">
@@ -2241,13 +2237,13 @@
       </c>
       <c r="E53" s="2" t="inlineStr">
         <is>
-          <t>Address Text</t>
+          <t>Postcode</t>
         </is>
       </c>
       <c r="F53" s="2" t="inlineStr"/>
       <c r="G53" s="2" t="inlineStr">
         <is>
-          <t>Flexible field for capturing addresses</t>
+          <t>The postal code</t>
         </is>
       </c>
       <c r="H53" s="2" t="inlineStr">
@@ -2257,32 +2253,32 @@
       </c>
       <c r="I53" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="n"/>
-      <c r="B54" s="2" t="n"/>
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>Checklist</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr">
+        <is>
+          <t>Checking whether all the requirements of the form have been met, such as proof of payment or supporting documentation.</t>
+        </is>
+      </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>Applicants[]</t>
-        </is>
-      </c>
-      <c r="D54" s="2" t="inlineStr">
-        <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E54" s="2" t="inlineStr">
-        <is>
-          <t>Postcode</t>
-        </is>
-      </c>
+          <t>National requirement types[]</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr"/>
+      <c r="E54" s="2" t="inlineStr"/>
       <c r="F54" s="2" t="inlineStr"/>
       <c r="G54" s="2" t="inlineStr">
         <is>
-          <t>The postal code</t>
+          <t>List of the document types required for the given application type</t>
         </is>
       </c>
       <c r="H54" s="2" t="inlineStr">
@@ -2292,24 +2288,24 @@
       </c>
       <c r="I54" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>Checklist</t>
+          <t>Community consultation</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
         <is>
-          <t>Checking whether all the requirements of the form have been met, such as proof of payment or supporting documentation.</t>
+          <t>What community consultation activities have taken place as part of the application</t>
         </is>
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>National requirement types[]</t>
+          <t>Have consulted</t>
         </is>
       </c>
       <c r="D55" s="2" t="inlineStr"/>
@@ -2317,12 +2313,12 @@
       <c r="F55" s="2" t="inlineStr"/>
       <c r="G55" s="2" t="inlineStr">
         <is>
-          <t>List of the document types required for the given application type</t>
+          <t>Whether community consultation has been carried out</t>
         </is>
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I55" s="2" t="inlineStr">
@@ -2332,19 +2328,11 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="inlineStr">
-        <is>
-          <t>Community consultation</t>
-        </is>
-      </c>
-      <c r="B56" s="2" t="inlineStr">
-        <is>
-          <t>What community consultation activities have taken place as part of the application</t>
-        </is>
-      </c>
+      <c r="A56" s="2" t="n"/>
+      <c r="B56" s="2" t="n"/>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>Have consulted</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr"/>
@@ -2352,26 +2340,34 @@
       <c r="F56" s="2" t="inlineStr"/>
       <c r="G56" s="2" t="inlineStr">
         <is>
-          <t>Whether community consultation has been carried out</t>
+          <t>Provide details of the community consultation</t>
         </is>
       </c>
       <c r="H56" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I56" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="n"/>
-      <c r="B57" s="2" t="n"/>
+      <c r="A57" s="2" t="inlineStr">
+        <is>
+          <t>Conflict of interest</t>
+        </is>
+      </c>
+      <c r="B57" s="2" t="inlineStr">
+        <is>
+          <t>Details of any conflict of interest that may exist between the applicant and planning authority.</t>
+        </is>
+      </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Conflict to declare</t>
         </is>
       </c>
       <c r="D57" s="2" t="inlineStr"/>
@@ -2379,34 +2375,26 @@
       <c r="F57" s="2" t="inlineStr"/>
       <c r="G57" s="2" t="inlineStr">
         <is>
-          <t>Provide details of the community consultation</t>
+          <t>Indicates whether any named applicant or agent has a relationship to the planning authority that must be declared</t>
         </is>
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I57" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="inlineStr">
-        <is>
-          <t>Conflict of interest</t>
-        </is>
-      </c>
-      <c r="B58" s="2" t="inlineStr">
-        <is>
-          <t>Details of any conflict of interest that may exist between the applicant and planning authority.</t>
-        </is>
-      </c>
+      <c r="A58" s="2" t="n"/>
+      <c r="B58" s="2" t="n"/>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>Conflict to declare</t>
+          <t>Conflict person name</t>
         </is>
       </c>
       <c r="D58" s="2" t="inlineStr"/>
@@ -2414,17 +2402,17 @@
       <c r="F58" s="2" t="inlineStr"/>
       <c r="G58" s="2" t="inlineStr">
         <is>
-          <t>Indicates whether any named applicant or agent has a relationship to the planning authority that must be declared</t>
+          <t>Name of the individual with the conflict of interest that matches one of the names provided in applicants/agent section</t>
         </is>
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I58" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -2433,7 +2421,7 @@
       <c r="B59" s="2" t="n"/>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>Conflict person name</t>
+          <t>Conflict details</t>
         </is>
       </c>
       <c r="D59" s="2" t="inlineStr"/>
@@ -2441,7 +2429,7 @@
       <c r="F59" s="2" t="inlineStr"/>
       <c r="G59" s="2" t="inlineStr">
         <is>
-          <t>Name of the individual with the conflict of interest that matches one of the names provided in applicants/agent section</t>
+          <t>Details of the conflict of interest including name, role and how the individual is related to the planning authority</t>
         </is>
       </c>
       <c r="H59" s="2" t="inlineStr">
@@ -2456,11 +2444,19 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2" t="n"/>
-      <c r="B60" s="2" t="n"/>
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>Interest in land</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="inlineStr">
+        <is>
+          <t>Whether the applicant owns or has permission to use the land where the proposed advertisement will be placed</t>
+        </is>
+      </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>Conflict details</t>
+          <t>Applicant owns land</t>
         </is>
       </c>
       <c r="D60" s="2" t="inlineStr"/>
@@ -2468,34 +2464,26 @@
       <c r="F60" s="2" t="inlineStr"/>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>Details of the conflict of interest including name, role and how the individual is related to the planning authority</t>
+          <t>True or False indicating whether the applicant owns the land where the advertisement will be displayed</t>
         </is>
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I60" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="inlineStr">
-        <is>
-          <t>Interest in land</t>
-        </is>
-      </c>
-      <c r="B61" s="2" t="inlineStr">
-        <is>
-          <t>Whether the applicant owns or has permission to use the land where the proposed advertisement will be placed</t>
-        </is>
-      </c>
+      <c r="A61" s="2" t="n"/>
+      <c r="B61" s="2" t="n"/>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>Applicant owns land</t>
+          <t>Permission obtained</t>
         </is>
       </c>
       <c r="D61" s="2" t="inlineStr"/>
@@ -2503,7 +2491,7 @@
       <c r="F61" s="2" t="inlineStr"/>
       <c r="G61" s="2" t="inlineStr">
         <is>
-          <t>True or False indicating whether the applicant owns the land where the advertisement will be displayed</t>
+          <t>True or False indicating whether permission of the owner for the display of an advertisement has been obtained</t>
         </is>
       </c>
       <c r="H61" s="2" t="inlineStr">
@@ -2513,7 +2501,7 @@
       </c>
       <c r="I61" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -2522,7 +2510,7 @@
       <c r="B62" s="2" t="n"/>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>Permission obtained</t>
+          <t>Permission not obtained details</t>
         </is>
       </c>
       <c r="D62" s="2" t="inlineStr"/>
@@ -2530,12 +2518,12 @@
       <c r="F62" s="2" t="inlineStr"/>
       <c r="G62" s="2" t="inlineStr">
         <is>
-          <t>True or False indicating whether permission of the owner for the display of an advertisement has been obtained</t>
+          <t>Details explaining why permission from the land owner has not been obtained for the advertisement display</t>
         </is>
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I62" s="2" t="inlineStr">
@@ -2545,11 +2533,19 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="n"/>
-      <c r="B63" s="2" t="n"/>
+      <c r="A63" s="2" t="inlineStr">
+        <is>
+          <t>Declaration</t>
+        </is>
+      </c>
+      <c r="B63" s="2" t="inlineStr">
+        <is>
+          <t>Signed and dated verification of the application's accuracy.</t>
+        </is>
+      </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>Permission not obtained details</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="D63" s="2" t="inlineStr"/>
@@ -2557,7 +2553,7 @@
       <c r="F63" s="2" t="inlineStr"/>
       <c r="G63" s="2" t="inlineStr">
         <is>
-          <t>Details explaining why permission from the land owner has not been obtained for the advertisement display</t>
+          <t>A name of a person</t>
         </is>
       </c>
       <c r="H63" s="2" t="inlineStr">
@@ -2567,24 +2563,16 @@
       </c>
       <c r="I63" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="inlineStr">
-        <is>
-          <t>Declaration</t>
-        </is>
-      </c>
-      <c r="B64" s="2" t="inlineStr">
-        <is>
-          <t>Signed and dated verification of the application's accuracy.</t>
-        </is>
-      </c>
+      <c r="A64" s="2" t="n"/>
+      <c r="B64" s="2" t="n"/>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Declaration confirmed</t>
         </is>
       </c>
       <c r="D64" s="2" t="inlineStr"/>
@@ -2592,12 +2580,12 @@
       <c r="F64" s="2" t="inlineStr"/>
       <c r="G64" s="2" t="inlineStr">
         <is>
-          <t>A name of a person</t>
+          <t>Confirms the applicant or agent has reviewed and validated the information provided in the application</t>
         </is>
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I64" s="2" t="inlineStr">
@@ -2611,7 +2599,7 @@
       <c r="B65" s="2" t="n"/>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>Declaration confirmed</t>
+          <t>Declaration date</t>
         </is>
       </c>
       <c r="D65" s="2" t="inlineStr"/>
@@ -2619,12 +2607,12 @@
       <c r="F65" s="2" t="inlineStr"/>
       <c r="G65" s="2" t="inlineStr">
         <is>
-          <t>Confirms the applicant or agent has reviewed and validated the information provided in the application</t>
+          <t>The date the declaration was made</t>
         </is>
       </c>
       <c r="H65" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I65" s="2" t="inlineStr">
@@ -2634,11 +2622,19 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="n"/>
-      <c r="B66" s="2" t="n"/>
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>Pre-application advice</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>Details of pre-application advice previously received from the planning authority</t>
+        </is>
+      </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>Declaration date</t>
+          <t>Pre-application advice sought</t>
         </is>
       </c>
       <c r="D66" s="2" t="inlineStr"/>
@@ -2646,12 +2642,12 @@
       <c r="F66" s="2" t="inlineStr"/>
       <c r="G66" s="2" t="inlineStr">
         <is>
-          <t>The date the declaration was made</t>
+          <t>Whether pre-application advice has been sought from the planning authority</t>
         </is>
       </c>
       <c r="H66" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I66" s="2" t="inlineStr">
@@ -2661,19 +2657,11 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="2" t="inlineStr">
-        <is>
-          <t>Pre-application advice</t>
-        </is>
-      </c>
-      <c r="B67" s="2" t="inlineStr">
-        <is>
-          <t>Details of pre-application advice previously received from the planning authority</t>
-        </is>
-      </c>
+      <c r="A67" s="2" t="n"/>
+      <c r="B67" s="2" t="n"/>
       <c r="C67" s="2" t="inlineStr">
         <is>
-          <t>Pre-application advice sought</t>
+          <t>Officer name</t>
         </is>
       </c>
       <c r="D67" s="2" t="inlineStr"/>
@@ -2681,17 +2669,17 @@
       <c r="F67" s="2" t="inlineStr"/>
       <c r="G67" s="2" t="inlineStr">
         <is>
-          <t>Whether pre-application advice has been sought from the planning authority</t>
+          <t>Name of the planning officer who provided the pre-application advice</t>
         </is>
       </c>
       <c r="H67" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I67" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -2700,7 +2688,7 @@
       <c r="B68" s="2" t="n"/>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>Officer name</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="D68" s="2" t="inlineStr"/>
@@ -2708,7 +2696,7 @@
       <c r="F68" s="2" t="inlineStr"/>
       <c r="G68" s="2" t="inlineStr">
         <is>
-          <t>Name of the planning officer who provided the pre-application advice</t>
+          <t>A unique reference for the data item</t>
         </is>
       </c>
       <c r="H68" s="2" t="inlineStr">
@@ -2727,7 +2715,7 @@
       <c r="B69" s="2" t="n"/>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>Reference</t>
+          <t>Advice date</t>
         </is>
       </c>
       <c r="D69" s="2" t="inlineStr"/>
@@ -2735,7 +2723,7 @@
       <c r="F69" s="2" t="inlineStr"/>
       <c r="G69" s="2" t="inlineStr">
         <is>
-          <t>A unique reference for the data item</t>
+          <t>Date when pre-application advice was received, in YYYY-MM-DD format</t>
         </is>
       </c>
       <c r="H69" s="2" t="inlineStr">
@@ -2754,7 +2742,7 @@
       <c r="B70" s="2" t="n"/>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>Advice date</t>
+          <t>Advice summary</t>
         </is>
       </c>
       <c r="D70" s="2" t="inlineStr"/>
@@ -2762,7 +2750,7 @@
       <c r="F70" s="2" t="inlineStr"/>
       <c r="G70" s="2" t="inlineStr">
         <is>
-          <t>Date when pre-application advice was received, in YYYY-MM-DD format</t>
+          <t>Summary of the pre-application advice received from the planning authority</t>
         </is>
       </c>
       <c r="H70" s="2" t="inlineStr">
@@ -2777,24 +2765,36 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="n"/>
-      <c r="B71" s="2" t="n"/>
+      <c r="A71" s="2" t="inlineStr">
+        <is>
+          <t>Proposed advert details</t>
+        </is>
+      </c>
+      <c r="B71" s="2" t="inlineStr">
+        <is>
+          <t>Details of the proposed advertisements such as their size and how they are made</t>
+        </is>
+      </c>
       <c r="C71" s="2" t="inlineStr">
         <is>
-          <t>Advice summary</t>
-        </is>
-      </c>
-      <c r="D71" s="2" t="inlineStr"/>
+          <t>Advertisements[]</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>Height from ground</t>
+        </is>
+      </c>
       <c r="E71" s="2" t="inlineStr"/>
       <c r="F71" s="2" t="inlineStr"/>
       <c r="G71" s="2" t="inlineStr">
         <is>
-          <t>Summary of the pre-application advice received from the planning authority</t>
+          <t>Height, in metres, from ground to the base of the advertisement</t>
         </is>
       </c>
       <c r="H71" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I71" s="2" t="inlineStr">
@@ -2804,16 +2804,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="inlineStr">
-        <is>
-          <t>Proposed advert details</t>
-        </is>
-      </c>
-      <c r="B72" s="2" t="inlineStr">
-        <is>
-          <t>Details of the proposed advertisements such as their size and how they are made</t>
-        </is>
-      </c>
+      <c r="A72" s="2" t="n"/>
+      <c r="B72" s="2" t="n"/>
       <c r="C72" s="2" t="inlineStr">
         <is>
           <t>Advertisements[]</t>
@@ -2821,14 +2813,14 @@
       </c>
       <c r="D72" s="2" t="inlineStr">
         <is>
-          <t>Height from ground</t>
+          <t>Height</t>
         </is>
       </c>
       <c r="E72" s="2" t="inlineStr"/>
       <c r="F72" s="2" t="inlineStr"/>
       <c r="G72" s="2" t="inlineStr">
         <is>
-          <t>Height, in metres, from ground to the base of the advertisement</t>
+          <t>Height, in metres, of dimensions of advertisement</t>
         </is>
       </c>
       <c r="H72" s="2" t="inlineStr">
@@ -2852,14 +2844,14 @@
       </c>
       <c r="D73" s="2" t="inlineStr">
         <is>
-          <t>Height</t>
+          <t>Width</t>
         </is>
       </c>
       <c r="E73" s="2" t="inlineStr"/>
       <c r="F73" s="2" t="inlineStr"/>
       <c r="G73" s="2" t="inlineStr">
         <is>
-          <t>Height, in metres, of dimensions of advertisement</t>
+          <t>Width of dimensions of advertisement</t>
         </is>
       </c>
       <c r="H73" s="2" t="inlineStr">
@@ -2883,14 +2875,14 @@
       </c>
       <c r="D74" s="2" t="inlineStr">
         <is>
-          <t>Width</t>
+          <t>Depth</t>
         </is>
       </c>
       <c r="E74" s="2" t="inlineStr"/>
       <c r="F74" s="2" t="inlineStr"/>
       <c r="G74" s="2" t="inlineStr">
         <is>
-          <t>Width of dimensions of advertisement</t>
+          <t>Depth, in metres, of dimensions of advertisement</t>
         </is>
       </c>
       <c r="H74" s="2" t="inlineStr">
@@ -2914,14 +2906,14 @@
       </c>
       <c r="D75" s="2" t="inlineStr">
         <is>
-          <t>Depth</t>
+          <t>Symbol height max</t>
         </is>
       </c>
       <c r="E75" s="2" t="inlineStr"/>
       <c r="F75" s="2" t="inlineStr"/>
       <c r="G75" s="2" t="inlineStr">
         <is>
-          <t>Depth, in metres, of dimensions of advertisement</t>
+          <t>Maximum height, in metres, of any individual letters or symbols</t>
         </is>
       </c>
       <c r="H75" s="2" t="inlineStr">
@@ -2945,19 +2937,19 @@
       </c>
       <c r="D76" s="2" t="inlineStr">
         <is>
-          <t>Symbol height max</t>
+          <t>Colour</t>
         </is>
       </c>
       <c r="E76" s="2" t="inlineStr"/>
       <c r="F76" s="2" t="inlineStr"/>
       <c r="G76" s="2" t="inlineStr">
         <is>
-          <t>Maximum height, in metres, of any individual letters or symbols</t>
+          <t>Colour of proposed sign</t>
         </is>
       </c>
       <c r="H76" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I76" s="2" t="inlineStr">
@@ -2976,14 +2968,14 @@
       </c>
       <c r="D77" s="2" t="inlineStr">
         <is>
-          <t>Colour</t>
+          <t>Materials</t>
         </is>
       </c>
       <c r="E77" s="2" t="inlineStr"/>
       <c r="F77" s="2" t="inlineStr"/>
       <c r="G77" s="2" t="inlineStr">
         <is>
-          <t>Colour of proposed sign</t>
+          <t>Materials of proposed sign</t>
         </is>
       </c>
       <c r="H77" s="2" t="inlineStr">
@@ -3007,19 +2999,19 @@
       </c>
       <c r="D78" s="2" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Max projection</t>
         </is>
       </c>
       <c r="E78" s="2" t="inlineStr"/>
       <c r="F78" s="2" t="inlineStr"/>
       <c r="G78" s="2" t="inlineStr">
         <is>
-          <t>Materials of proposed sign</t>
+          <t>Maximum projection, in metres, of the advertisement from the face of the building</t>
         </is>
       </c>
       <c r="H78" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I78" s="2" t="inlineStr">
@@ -3038,19 +3030,19 @@
       </c>
       <c r="D79" s="2" t="inlineStr">
         <is>
-          <t>Max projection</t>
+          <t>Illuminated</t>
         </is>
       </c>
       <c r="E79" s="2" t="inlineStr"/>
       <c r="F79" s="2" t="inlineStr"/>
       <c r="G79" s="2" t="inlineStr">
         <is>
-          <t>Maximum projection, in metres, of the advertisement from the face of the building</t>
+          <t>Will the sign(s) be illuminated?</t>
         </is>
       </c>
       <c r="H79" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I79" s="2" t="inlineStr">
@@ -3069,19 +3061,19 @@
       </c>
       <c r="D80" s="2" t="inlineStr">
         <is>
-          <t>Illuminated</t>
+          <t>Illumination method</t>
         </is>
       </c>
       <c r="E80" s="2" t="inlineStr"/>
       <c r="F80" s="2" t="inlineStr"/>
       <c r="G80" s="2" t="inlineStr">
         <is>
-          <t>Will the sign(s) be illuminated?</t>
+          <t>Method of illumination for the advertisement</t>
         </is>
       </c>
       <c r="H80" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I80" s="2" t="inlineStr">
@@ -3100,19 +3092,19 @@
       </c>
       <c r="D81" s="2" t="inlineStr">
         <is>
-          <t>Illumination method</t>
+          <t>Illuminance level</t>
         </is>
       </c>
       <c r="E81" s="2" t="inlineStr"/>
       <c r="F81" s="2" t="inlineStr"/>
       <c r="G81" s="2" t="inlineStr">
         <is>
-          <t>Method of illumination for the advertisement</t>
+          <t>Level of illuminance for the advertisement</t>
         </is>
       </c>
       <c r="H81" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I81" s="2" t="inlineStr">
@@ -3131,19 +3123,19 @@
       </c>
       <c r="D82" s="2" t="inlineStr">
         <is>
-          <t>Illuminance level</t>
+          <t>Illumination type</t>
         </is>
       </c>
       <c r="E82" s="2" t="inlineStr"/>
       <c r="F82" s="2" t="inlineStr"/>
       <c r="G82" s="2" t="inlineStr">
         <is>
-          <t>Level of illuminance for the advertisement</t>
+          <t>Type of illumination (static or intermittent)</t>
         </is>
       </c>
       <c r="H82" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I82" s="2" t="inlineStr">
@@ -3153,28 +3145,36 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="2" t="n"/>
-      <c r="B83" s="2" t="n"/>
+      <c r="A83" s="2" t="inlineStr">
+        <is>
+          <t>Site details</t>
+        </is>
+      </c>
+      <c r="B83" s="2" t="inlineStr">
+        <is>
+          <t>Where the proposed development will be built.</t>
+        </is>
+      </c>
       <c r="C83" s="2" t="inlineStr">
         <is>
-          <t>Advertisements[]</t>
+          <t>Site locations[]</t>
         </is>
       </c>
       <c r="D83" s="2" t="inlineStr">
         <is>
-          <t>Illumination type</t>
+          <t>Site boundary</t>
         </is>
       </c>
       <c r="E83" s="2" t="inlineStr"/>
       <c r="F83" s="2" t="inlineStr"/>
       <c r="G83" s="2" t="inlineStr">
         <is>
-          <t>Type of illumination (static or intermittent)</t>
+          <t>Geometry of the site of the development, typically in GeoJSON format</t>
         </is>
       </c>
       <c r="H83" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>wkt</t>
         </is>
       </c>
       <c r="I83" s="2" t="inlineStr">
@@ -3184,16 +3184,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="inlineStr">
-        <is>
-          <t>Site details</t>
-        </is>
-      </c>
-      <c r="B84" s="2" t="inlineStr">
-        <is>
-          <t>Where the proposed development will be built.</t>
-        </is>
-      </c>
+      <c r="A84" s="2" t="n"/>
+      <c r="B84" s="2" t="n"/>
       <c r="C84" s="2" t="inlineStr">
         <is>
           <t>Site locations[]</t>
@@ -3201,19 +3193,19 @@
       </c>
       <c r="D84" s="2" t="inlineStr">
         <is>
-          <t>Site boundary</t>
+          <t>Address Text</t>
         </is>
       </c>
       <c r="E84" s="2" t="inlineStr"/>
       <c r="F84" s="2" t="inlineStr"/>
       <c r="G84" s="2" t="inlineStr">
         <is>
-          <t>Geometry of the site of the development, typically in GeoJSON format</t>
+          <t>Flexible field for capturing addresses</t>
         </is>
       </c>
       <c r="H84" s="2" t="inlineStr">
         <is>
-          <t>wkt</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I84" s="2" t="inlineStr">
@@ -3232,14 +3224,14 @@
       </c>
       <c r="D85" s="2" t="inlineStr">
         <is>
-          <t>Address Text</t>
+          <t>Postcode</t>
         </is>
       </c>
       <c r="E85" s="2" t="inlineStr"/>
       <c r="F85" s="2" t="inlineStr"/>
       <c r="G85" s="2" t="inlineStr">
         <is>
-          <t>Flexible field for capturing addresses</t>
+          <t>The postal code</t>
         </is>
       </c>
       <c r="H85" s="2" t="inlineStr">
@@ -3263,19 +3255,19 @@
       </c>
       <c r="D86" s="2" t="inlineStr">
         <is>
-          <t>Postcode</t>
+          <t>Easting</t>
         </is>
       </c>
       <c r="E86" s="2" t="inlineStr"/>
       <c r="F86" s="2" t="inlineStr"/>
       <c r="G86" s="2" t="inlineStr">
         <is>
-          <t>The postal code</t>
+          <t>Easting coordinate in British National Grid (EPSG:27700)</t>
         </is>
       </c>
       <c r="H86" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I86" s="2" t="inlineStr">
@@ -3294,14 +3286,14 @@
       </c>
       <c r="D87" s="2" t="inlineStr">
         <is>
-          <t>Easting</t>
+          <t>Northing</t>
         </is>
       </c>
       <c r="E87" s="2" t="inlineStr"/>
       <c r="F87" s="2" t="inlineStr"/>
       <c r="G87" s="2" t="inlineStr">
         <is>
-          <t>Easting coordinate in British National Grid (EPSG:27700)</t>
+          <t>Northing coordinate in British National Grid (EPSG:27700)</t>
         </is>
       </c>
       <c r="H87" s="2" t="inlineStr">
@@ -3325,14 +3317,14 @@
       </c>
       <c r="D88" s="2" t="inlineStr">
         <is>
-          <t>Northing</t>
+          <t>Latitude</t>
         </is>
       </c>
       <c r="E88" s="2" t="inlineStr"/>
       <c r="F88" s="2" t="inlineStr"/>
       <c r="G88" s="2" t="inlineStr">
         <is>
-          <t>Northing coordinate in British National Grid (EPSG:27700)</t>
+          <t>Latitude coordinate in WGS84 (EPSG:4326)</t>
         </is>
       </c>
       <c r="H88" s="2" t="inlineStr">
@@ -3356,14 +3348,14 @@
       </c>
       <c r="D89" s="2" t="inlineStr">
         <is>
-          <t>Latitude</t>
+          <t>Longitude</t>
         </is>
       </c>
       <c r="E89" s="2" t="inlineStr"/>
       <c r="F89" s="2" t="inlineStr"/>
       <c r="G89" s="2" t="inlineStr">
         <is>
-          <t>Latitude coordinate in WGS84 (EPSG:4326)</t>
+          <t>Longitude coordinate in WGS84 (EPSG:4326)</t>
         </is>
       </c>
       <c r="H89" s="2" t="inlineStr">
@@ -3387,19 +3379,19 @@
       </c>
       <c r="D90" s="2" t="inlineStr">
         <is>
-          <t>Longitude</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="E90" s="2" t="inlineStr"/>
       <c r="F90" s="2" t="inlineStr"/>
       <c r="G90" s="2" t="inlineStr">
         <is>
-          <t>Longitude coordinate in WGS84 (EPSG:4326)</t>
+          <t>A text description providing details about the subject. For parking changes, this describes how the proposed works affect existing car parking arrangements.</t>
         </is>
       </c>
       <c r="H90" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I90" s="2" t="inlineStr">
@@ -3418,14 +3410,14 @@
       </c>
       <c r="D91" s="2" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>UPRNs[]</t>
         </is>
       </c>
       <c r="E91" s="2" t="inlineStr"/>
       <c r="F91" s="2" t="inlineStr"/>
       <c r="G91" s="2" t="inlineStr">
         <is>
-          <t>A text description providing details about the subject. For parking changes, this describes how the proposed works affect existing car parking arrangements.</t>
+          <t>Unique Property Reference Numbers (UPRNs) for properties within the site boundary</t>
         </is>
       </c>
       <c r="H91" s="2" t="inlineStr">
@@ -3440,50 +3432,46 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="n"/>
-      <c r="B92" s="2" t="n"/>
+      <c r="A92" s="2" t="inlineStr">
+        <is>
+          <t>Site Visit Details</t>
+        </is>
+      </c>
+      <c r="B92" s="2" t="inlineStr">
+        <is>
+          <t>Information to help the planning authority arrange a site visit</t>
+        </is>
+      </c>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>Site locations[]</t>
-        </is>
-      </c>
-      <c r="D92" s="2" t="inlineStr">
-        <is>
-          <t>UPRNs[]</t>
-        </is>
-      </c>
+          <t>Site seen from public area</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="inlineStr"/>
       <c r="E92" s="2" t="inlineStr"/>
       <c r="F92" s="2" t="inlineStr"/>
       <c r="G92" s="2" t="inlineStr">
         <is>
-          <t>Unique Property Reference Numbers (UPRNs) for properties within the site boundary</t>
+          <t>Can site be seen from a public road, public footpath, bridleway or other public land</t>
         </is>
       </c>
       <c r="H92" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I92" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="inlineStr">
-        <is>
-          <t>Site Visit Details</t>
-        </is>
-      </c>
-      <c r="B93" s="2" t="inlineStr">
-        <is>
-          <t>Information to help the planning authority arrange a site visit</t>
-        </is>
-      </c>
+      <c r="A93" s="2" t="n"/>
+      <c r="B93" s="2" t="n"/>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>Site seen from public area</t>
+          <t>Site visit contact type</t>
         </is>
       </c>
       <c r="D93" s="2" t="inlineStr"/>
@@ -3491,12 +3479,12 @@
       <c r="F93" s="2" t="inlineStr"/>
       <c r="G93" s="2" t="inlineStr">
         <is>
-          <t>Can site be seen from a public road, public footpath, bridleway or other public land</t>
+          <t>Indicates who the authority should contact to arrange a site visit</t>
         </is>
       </c>
       <c r="H93" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I93" s="2" t="inlineStr">
@@ -3510,7 +3498,7 @@
       <c r="B94" s="2" t="n"/>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>Site visit contact type</t>
+          <t>Contact reference</t>
         </is>
       </c>
       <c r="D94" s="2" t="inlineStr"/>
@@ -3518,17 +3506,17 @@
       <c r="F94" s="2" t="inlineStr"/>
       <c r="G94" s="2" t="inlineStr">
         <is>
-          <t>Indicates who the authority should contact to arrange a site visit</t>
+          <t>The reference of the applicant or agent who should be contacted for site visits</t>
         </is>
       </c>
       <c r="H94" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I94" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -3537,15 +3525,19 @@
       <c r="B95" s="2" t="n"/>
       <c r="C95" s="2" t="inlineStr">
         <is>
-          <t>Contact reference</t>
-        </is>
-      </c>
-      <c r="D95" s="2" t="inlineStr"/>
+          <t>Other site visit contact</t>
+        </is>
+      </c>
+      <c r="D95" s="2" t="inlineStr">
+        <is>
+          <t>Full name</t>
+        </is>
+      </c>
       <c r="E95" s="2" t="inlineStr"/>
       <c r="F95" s="2" t="inlineStr"/>
       <c r="G95" s="2" t="inlineStr">
         <is>
-          <t>The reference of the applicant or agent who should be contacted for site visits</t>
+          <t>The complete name of a person</t>
         </is>
       </c>
       <c r="H95" s="2" t="inlineStr">
@@ -3555,7 +3547,7 @@
       </c>
       <c r="I95" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -3569,14 +3561,14 @@
       </c>
       <c r="D96" s="2" t="inlineStr">
         <is>
-          <t>Full name</t>
+          <t>Phone number</t>
         </is>
       </c>
       <c r="E96" s="2" t="inlineStr"/>
       <c r="F96" s="2" t="inlineStr"/>
       <c r="G96" s="2" t="inlineStr">
         <is>
-          <t>The complete name of a person</t>
+          <t>A phone number</t>
         </is>
       </c>
       <c r="H96" s="2" t="inlineStr">
@@ -3600,14 +3592,14 @@
       </c>
       <c r="D97" s="2" t="inlineStr">
         <is>
-          <t>Phone number</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="E97" s="2" t="inlineStr"/>
       <c r="F97" s="2" t="inlineStr"/>
       <c r="G97" s="2" t="inlineStr">
         <is>
-          <t>A phone number</t>
+          <t>The email address that can be used for electronic correspondence with the individual</t>
         </is>
       </c>
       <c r="H97" s="2" t="inlineStr">
@@ -3616,37 +3608,6 @@
         </is>
       </c>
       <c r="I97" s="2" t="inlineStr">
-        <is>
-          <t>MUST</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="2" t="n"/>
-      <c r="B98" s="2" t="n"/>
-      <c r="C98" s="2" t="inlineStr">
-        <is>
-          <t>Other site visit contact</t>
-        </is>
-      </c>
-      <c r="D98" s="2" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="E98" s="2" t="inlineStr"/>
-      <c r="F98" s="2" t="inlineStr"/>
-      <c r="G98" s="2" t="inlineStr">
-        <is>
-          <t>The email address that can be used for electronic correspondence with the individual</t>
-        </is>
-      </c>
-      <c r="H98" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I98" s="2" t="inlineStr">
         <is>
           <t>MUST</t>
         </is>
@@ -3654,40 +3615,40 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B55"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B93:B98"/>
-    <mergeCell ref="B84:B92"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B2:B20"/>
-    <mergeCell ref="B72:B83"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A37:A44"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B37:B44"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="A2:A20"/>
-    <mergeCell ref="A55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A72:A83"/>
-    <mergeCell ref="A93:A98"/>
-    <mergeCell ref="A84:A92"/>
+    <mergeCell ref="A48:A53"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A92:A97"/>
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="B48:B53"/>
+    <mergeCell ref="B83:B91"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B54"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B71:B82"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B66:B70"/>
+    <mergeCell ref="A83:A91"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A66:A70"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B92:B97"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="A71:A82"/>
+    <mergeCell ref="B2:B19"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B36:B43"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest generated outputs 2026-01-14
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/advertising-advertising.xlsx
+++ b/generated/spreadsheet/advertising-advertising.xlsx
@@ -842,27 +842,23 @@
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>File</t>
-        </is>
-      </c>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>Base64</t>
-        </is>
-      </c>
+          <t>Uploaded date</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr"/>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>Base64-encoded content of the file for inline file uploads</t>
+          <t>The date the document was uploaded to the application</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>date</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -886,12 +882,12 @@
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>Filename</t>
+          <t>Base64</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Name of the file being uploaded</t>
+          <t>Base64-encoded content of the file for inline file uploads</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
@@ -901,7 +897,7 @@
       </c>
       <c r="I13" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -925,12 +921,12 @@
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>MIME type</t>
+          <t>Filename</t>
         </is>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>The file's MIME type such as application/pdf or image/jpeg</t>
+          <t>Name of the file being uploaded</t>
         </is>
       </c>
       <c r="H14" s="2" t="inlineStr">
@@ -940,7 +936,7 @@
       </c>
       <c r="I14" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -964,17 +960,17 @@
       </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>File size</t>
+          <t>MIME type</t>
         </is>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Size of the file in bytes that can be used to enforce limits</t>
+          <t>The file's MIME type such as application/pdf or image/jpeg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I15" s="2" t="inlineStr">
@@ -993,18 +989,22 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>Fee</t>
+          <t>Documents[]</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Amount</t>
-        </is>
-      </c>
-      <c r="F16" s="2" t="inlineStr"/>
+          <t>File</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>File size</t>
+        </is>
+      </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>The total amount due for the application fee</t>
+          <t>Size of the file in bytes that can be used to enforce limits</t>
         </is>
       </c>
       <c r="H16" s="2" t="inlineStr">
@@ -1014,7 +1014,7 @@
       </c>
       <c r="I16" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -1033,13 +1033,13 @@
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>Amount paid</t>
+          <t>Amount</t>
         </is>
       </c>
       <c r="F17" s="2" t="inlineStr"/>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>The amount paid towards the application fee</t>
+          <t>The total amount due for the application fee</t>
         </is>
       </c>
       <c r="H17" s="2" t="inlineStr">
@@ -1068,67 +1068,75 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Transactions[]</t>
+          <t>Amount paid</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr"/>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>References to payments or financial transactions related to this application</t>
+          <t>The amount paid towards the application fee</t>
         </is>
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I18" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>Advertisement location</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>Where the advertisement being applied to be built will be located</t>
-        </is>
-      </c>
+      <c r="A19" s="2" t="n"/>
+      <c r="B19" s="2" t="n"/>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>Is advert in place</t>
-        </is>
-      </c>
-      <c r="D19" s="2" t="inlineStr"/>
-      <c r="E19" s="2" t="inlineStr"/>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>Fee</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>Transactions[]</t>
+        </is>
+      </c>
       <c r="F19" s="2" t="inlineStr"/>
       <c r="G19" s="2" t="inlineStr">
         <is>
-          <t>Whether the advertisement is already in place</t>
+          <t>References to payments or financial transactions related to this application</t>
         </is>
       </c>
       <c r="H19" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I19" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n"/>
-      <c r="B20" s="2" t="n"/>
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>Advertisement location</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>Where the advertisement being applied to be built will be located</t>
+        </is>
+      </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Advert placed date</t>
+          <t>Is advert in place</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr"/>
@@ -1136,17 +1144,17 @@
       <c r="F20" s="2" t="inlineStr"/>
       <c r="G20" s="2" t="inlineStr">
         <is>
-          <t>Date when the advertisement was placed (YYYY-MM-DD format)</t>
+          <t>Whether the advertisement is already in place</t>
         </is>
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I20" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1163,7 @@
       <c r="B21" s="2" t="n"/>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Is replacement advert</t>
+          <t>Advert placed date</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr"/>
@@ -1163,17 +1171,17 @@
       <c r="F21" s="2" t="inlineStr"/>
       <c r="G21" s="2" t="inlineStr">
         <is>
-          <t>Whether this is a replacement advertisement</t>
+          <t>Date when the advertisement was placed (YYYY-MM-DD format)</t>
         </is>
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>date</t>
         </is>
       </c>
       <c r="I21" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -1182,24 +1190,20 @@
       <c r="B22" s="2" t="n"/>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Document reference[]</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
+          <t>Is replacement advert</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr"/>
       <c r="E22" s="2" t="inlineStr"/>
       <c r="F22" s="2" t="inlineStr"/>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>A unique reference for the data item</t>
+          <t>Whether this is a replacement advertisement</t>
         </is>
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I22" s="2" t="inlineStr">
@@ -1218,14 +1222,14 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="E23" s="2" t="inlineStr"/>
       <c r="F23" s="2" t="inlineStr"/>
       <c r="G23" s="2" t="inlineStr">
         <is>
-          <t>A name for the document. For example, The Site Plan</t>
+          <t>A unique reference for the data item</t>
         </is>
       </c>
       <c r="H23" s="2" t="inlineStr">
@@ -3034,7 +3038,7 @@
       </c>
       <c r="H79" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I79" s="2" t="inlineStr">
@@ -3583,23 +3587,23 @@
     <mergeCell ref="B91:B96"/>
     <mergeCell ref="B65:B69"/>
     <mergeCell ref="B82:B90"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A2:A19"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B2:B18"/>
     <mergeCell ref="B47:B52"/>
     <mergeCell ref="A59:A61"/>
     <mergeCell ref="B43:B46"/>
     <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B20:B24"/>
     <mergeCell ref="B56:B58"/>
     <mergeCell ref="B59:B61"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="B62:B64"/>
     <mergeCell ref="A70:A81"/>
-    <mergeCell ref="A2:A18"/>
     <mergeCell ref="A91:A96"/>
     <mergeCell ref="A82:A90"/>
-    <mergeCell ref="B19:B24"/>
     <mergeCell ref="A47:A52"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="B70:B81"/>
@@ -3608,7 +3612,7 @@
     <mergeCell ref="B53"/>
     <mergeCell ref="A65:A69"/>
     <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="B2:B19"/>
     <mergeCell ref="A56:A58"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Latest generated outputs 2026-01-26
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/advertising-advertising.xlsx
+++ b/generated/spreadsheet/advertising-advertising.xlsx
@@ -647,7 +647,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>datetime</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>datetime</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>datetime</t>
         </is>
       </c>
       <c r="I21" s="2" t="inlineStr">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>datetime</t>
         </is>
       </c>
       <c r="I25" s="2" t="inlineStr">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>datetime</t>
         </is>
       </c>
       <c r="I26" s="2" t="inlineStr">

</xml_diff>